<commit_message>
[doc]: change asvs cehck list
</commit_message>
<xml_diff>
--- a/Deliverables/v4-ASVS-checklist-en.xlsx
+++ b/Deliverables/v4-ASVS-checklist-en.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="ASVS Results" sheetId="1" state="visible" r:id="rId3"/>
@@ -3996,25 +3996,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>60</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>73.9130434782609</c:v>
+                  <c:v>85.7142857142857</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>66.3636363636364</c:v>
+                  <c:v>68.0555555555556</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="73049514"/>
-        <c:axId val="22751093"/>
+        <c:axId val="7201856"/>
+        <c:axId val="24155232"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="73049514"/>
+        <c:axId val="7201856"/>
         <c:scaling>
-          <c:orientation val="minMax"/>
+          <c:orientation val="maxMin"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -4051,7 +4051,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22751093"/>
+        <c:crossAx val="24155232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4059,7 +4059,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="22751093"/>
+        <c:axId val="24155232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4101,7 +4101,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73049514"/>
+        <c:crossAx val="7201856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4166,9 +4166,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1716840</xdr:colOff>
+      <xdr:colOff>1716480</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>23400</xdr:rowOff>
+      <xdr:rowOff>23040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4177,7 +4177,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="4293360"/>
-        <a:ext cx="11130120" cy="9331920"/>
+        <a:ext cx="11129760" cy="9331560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4627,11 +4627,11 @@
       </c>
       <c r="C14" s="8" t="n">
         <f aca="false">COUNTIF('API and Web Service'!G2:G16,"&lt;&gt;Not Applicable")</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D14" s="9" t="n">
         <f aca="false">(B14/C14)*100</f>
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="E14" s="10"/>
     </row>
@@ -4641,15 +4641,15 @@
       </c>
       <c r="B15" s="7" t="n">
         <f aca="false">COUNTIF(Configuration!G2:G26,"Valid")</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C15" s="8" t="n">
         <f aca="false">COUNTIF(Configuration!G2:G26,"&lt;&gt;Not Applicable")</f>
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D15" s="9" t="n">
         <f aca="false">(B15/C15)*100</f>
-        <v>73.9130434782609</v>
+        <v>85.7142857142857</v>
       </c>
       <c r="E15" s="10"/>
     </row>
@@ -4659,15 +4659,15 @@
       </c>
       <c r="B16" s="7" t="n">
         <f aca="false">SUM(B2:B15)</f>
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C16" s="8" t="n">
         <f aca="false">SUM(C2:C15)</f>
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D16" s="9" t="n">
         <f aca="false">(B16/C16)*100</f>
-        <v>66.3636363636364</v>
+        <v>68.0555555555556</v>
       </c>
       <c r="E16" s="10"/>
     </row>
@@ -4947,8 +4947,8 @@
   </sheetPr>
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5266,7 +5266,7 @@
   </sheetPr>
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -5520,7 +5520,7 @@
   </sheetPr>
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
     </sheetView>
   </sheetViews>
@@ -5911,8 +5911,8 @@
   </sheetPr>
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6145,7 +6145,7 @@
         <v>687</v>
       </c>
       <c r="G9" s="29" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
       <c r="H9" s="29"/>
       <c r="I9" s="29"/>
@@ -6285,7 +6285,7 @@
         <v>703</v>
       </c>
       <c r="G15" s="29" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
       <c r="H15" s="29"/>
       <c r="I15" s="29"/>
@@ -6343,8 +6343,8 @@
   </sheetPr>
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I25" activeCellId="0" sqref="I25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6776,7 +6776,7 @@
         <v>760</v>
       </c>
       <c r="G17" s="107" t="s">
-        <v>90</v>
+        <v>26</v>
       </c>
       <c r="H17" s="107" t="s">
         <v>761</v>
@@ -6800,7 +6800,7 @@
         <v>763</v>
       </c>
       <c r="G18" s="107" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
       <c r="H18" s="107"/>
       <c r="I18" s="107"/>
@@ -6896,7 +6896,7 @@
         <v>775</v>
       </c>
       <c r="G22" s="107" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
       <c r="H22" s="107"/>
       <c r="I22" s="107"/>
@@ -8205,7 +8205,7 @@
   </sheetPr>
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I52" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G58" activeCellId="0" sqref="G58"/>
     </sheetView>
   </sheetViews>
@@ -11744,7 +11744,7 @@
   </sheetPr>
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -12116,8 +12116,8 @@
   </sheetPr>
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
#8 [feat]: add list of used methods asvs - 14.5.1
</commit_message>
<xml_diff>
--- a/Deliverables/v4-ASVS-checklist-en.xlsx
+++ b/Deliverables/v4-ASVS-checklist-en.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="ASVS Results" sheetId="1" state="visible" r:id="rId3"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1244" uniqueCount="789">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1245" uniqueCount="790">
   <si>
     <t xml:space="preserve">Security Category</t>
   </si>
@@ -2405,6 +2405,10 @@
   </si>
   <si>
     <t xml:space="preserve">Verify that the application server only accepts the HTTP methods in use by the application/API, including pre-flight OPTIONS, and logs/alerts on any requests that are not valid for the application context.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Na api foi definido o uso de métodos específicos, que são os usados, como os métodos primitidos. 
+Isto pode ser visto no ficheiro SecurityConfig.java  linha 93</t>
   </si>
   <si>
     <t xml:space="preserve">14.5.2</t>
@@ -3257,7 +3261,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="118">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3706,6 +3710,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="43" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="5" borderId="45" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3999,22 +4007,22 @@
                   <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>85.7142857142857</c:v>
+                  <c:v>90.4761904761905</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>68.0555555555556</c:v>
+                  <c:v>68.5185185185185</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="7201856"/>
-        <c:axId val="24155232"/>
+        <c:axId val="16954317"/>
+        <c:axId val="73086819"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="7201856"/>
+        <c:axId val="16954317"/>
         <c:scaling>
-          <c:orientation val="maxMin"/>
+          <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -4051,7 +4059,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="24155232"/>
+        <c:crossAx val="73086819"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4059,7 +4067,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="24155232"/>
+        <c:axId val="73086819"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4101,7 +4109,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7201856"/>
+        <c:crossAx val="16954317"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4166,9 +4174,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1716480</xdr:colOff>
+      <xdr:colOff>1716120</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>23040</xdr:rowOff>
+      <xdr:rowOff>22680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4177,7 +4185,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="4293360"/>
-        <a:ext cx="11129760" cy="9331560"/>
+        <a:ext cx="11129400" cy="9331200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4641,7 +4649,7 @@
       </c>
       <c r="B15" s="7" t="n">
         <f aca="false">COUNTIF(Configuration!G2:G26,"Valid")</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C15" s="8" t="n">
         <f aca="false">COUNTIF(Configuration!G2:G26,"&lt;&gt;Not Applicable")</f>
@@ -4649,7 +4657,7 @@
       </c>
       <c r="D15" s="9" t="n">
         <f aca="false">(B15/C15)*100</f>
-        <v>85.7142857142857</v>
+        <v>90.4761904761905</v>
       </c>
       <c r="E15" s="10"/>
     </row>
@@ -4659,7 +4667,7 @@
       </c>
       <c r="B16" s="7" t="n">
         <f aca="false">SUM(B2:B15)</f>
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C16" s="8" t="n">
         <f aca="false">SUM(C2:C15)</f>
@@ -4667,7 +4675,7 @@
       </c>
       <c r="D16" s="9" t="n">
         <f aca="false">(B16/C16)*100</f>
-        <v>68.0555555555556</v>
+        <v>68.5185185185185</v>
       </c>
       <c r="E16" s="10"/>
     </row>
@@ -6343,8 +6351,8 @@
   </sheetPr>
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6616,7 +6624,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="48"/>
       <c r="B11" s="68" t="s">
         <v>740</v>
@@ -6920,16 +6928,18 @@
         <v>778</v>
       </c>
       <c r="G23" s="107" t="s">
-        <v>90</v>
-      </c>
-      <c r="H23" s="107"/>
+        <v>26</v>
+      </c>
+      <c r="H23" s="112" t="s">
+        <v>779</v>
+      </c>
       <c r="I23" s="107"/>
       <c r="J23" s="108"/>
     </row>
     <row r="24" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="48"/>
       <c r="B24" s="68" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="C24" s="111" t="n">
         <v>1</v>
@@ -6939,13 +6949,13 @@
       </c>
       <c r="E24" s="105"/>
       <c r="F24" s="106" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="G24" s="107" t="s">
         <v>26</v>
       </c>
       <c r="H24" s="107" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="I24" s="107"/>
       <c r="J24" s="108"/>
@@ -6953,7 +6963,7 @@
     <row r="25" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="48"/>
       <c r="B25" s="68" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="C25" s="111" t="n">
         <v>1</v>
@@ -6963,13 +6973,13 @@
       </c>
       <c r="E25" s="105"/>
       <c r="F25" s="106" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="G25" s="107" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="H25" s="107" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="I25" s="107"/>
       <c r="J25" s="108"/>
@@ -6977,26 +6987,26 @@
     <row r="26" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="48"/>
       <c r="B26" s="68" t="s">
-        <v>786</v>
-      </c>
-      <c r="C26" s="112" t="n">
-        <v>2</v>
-      </c>
-      <c r="D26" s="113" t="n">
+        <v>787</v>
+      </c>
+      <c r="C26" s="113" t="n">
+        <v>2</v>
+      </c>
+      <c r="D26" s="114" t="n">
         <v>306</v>
       </c>
-      <c r="E26" s="113"/>
-      <c r="F26" s="114" t="s">
-        <v>787</v>
-      </c>
-      <c r="G26" s="115" t="s">
-        <v>26</v>
-      </c>
-      <c r="H26" s="115" t="s">
+      <c r="E26" s="114"/>
+      <c r="F26" s="115" t="s">
         <v>788</v>
       </c>
-      <c r="I26" s="115"/>
-      <c r="J26" s="116"/>
+      <c r="G26" s="116" t="s">
+        <v>26</v>
+      </c>
+      <c r="H26" s="116" t="s">
+        <v>789</v>
+      </c>
+      <c r="I26" s="116"/>
+      <c r="J26" s="117"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -11744,7 +11754,7 @@
   </sheetPr>
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
#35 [feat]: add feature for user to delete its data on demand asvs - 8.3.2
</commit_message>
<xml_diff>
--- a/Deliverables/v4-ASVS-checklist-en.xlsx
+++ b/Deliverables/v4-ASVS-checklist-en.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="14"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="ASVS Results" sheetId="1" state="visible" r:id="rId3"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1245" uniqueCount="790">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1246" uniqueCount="791">
   <si>
     <t xml:space="preserve">Security Category</t>
   </si>
@@ -1711,6 +1711,10 @@
   </si>
   <si>
     <t xml:space="preserve">Verify that users have a method to remove or export their data on demand.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No user controller foi adicionado a request para apagar os dados do utilizador a pedido, UserController.java linha 33. isto pertence à issue #35
+</t>
   </si>
   <si>
     <t xml:space="preserve">8.3.3</t>
@@ -3989,7 +3993,7 @@
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>60</c:v>
+                  <c:v>73.3333333333333</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>100</c:v>
@@ -3998,29 +4002,29 @@
                   <c:v>88.8888888888889</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>50</c:v>
+                  <c:v>57.1428571428571</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>75</c:v>
+                  <c:v>85.7142857142857</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>90.4761904761905</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>68.5185185185185</c:v>
+                  <c:v>70.0934579439252</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="16954317"/>
-        <c:axId val="73086819"/>
+        <c:axId val="44868616"/>
+        <c:axId val="53282369"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="16954317"/>
+        <c:axId val="44868616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4059,7 +4063,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73086819"/>
+        <c:crossAx val="53282369"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4067,7 +4071,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="73086819"/>
+        <c:axId val="53282369"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4109,7 +4113,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="16954317"/>
+        <c:crossAx val="44868616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4541,7 +4545,7 @@
       </c>
       <c r="B9" s="7" t="n">
         <f aca="false">COUNTIF('Data Protection'!G2:G18,"Valid")</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C9" s="8" t="n">
         <f aca="false">COUNTIF('Data Protection'!G2:G18,"&lt;&gt;Not Applicable")</f>
@@ -4549,7 +4553,7 @@
       </c>
       <c r="D9" s="9" t="n">
         <f aca="false">(B9/C9)*100</f>
-        <v>60</v>
+        <v>73.3333333333333</v>
       </c>
       <c r="E9" s="10"/>
     </row>
@@ -4599,11 +4603,11 @@
       </c>
       <c r="C12" s="8" t="n">
         <f aca="false">COUNTIF('Business Logic'!G2:G9,"&lt;&gt;Not Applicable")</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D12" s="9" t="n">
         <f aca="false">(B12/C12)*100</f>
-        <v>50</v>
+        <v>57.1428571428571</v>
       </c>
       <c r="E12" s="10"/>
     </row>
@@ -4635,11 +4639,11 @@
       </c>
       <c r="C14" s="8" t="n">
         <f aca="false">COUNTIF('API and Web Service'!G2:G16,"&lt;&gt;Not Applicable")</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14" s="9" t="n">
         <f aca="false">(B14/C14)*100</f>
-        <v>75</v>
+        <v>85.7142857142857</v>
       </c>
       <c r="E14" s="10"/>
     </row>
@@ -4667,15 +4671,15 @@
       </c>
       <c r="B16" s="7" t="n">
         <f aca="false">SUM(B2:B15)</f>
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C16" s="8" t="n">
         <f aca="false">SUM(C2:C15)</f>
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D16" s="9" t="n">
         <f aca="false">(B16/C16)*100</f>
-        <v>68.5185185185185</v>
+        <v>70.0934579439252</v>
       </c>
       <c r="E16" s="10"/>
     </row>
@@ -4749,10 +4753,10 @@
     </row>
     <row r="2" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="48" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="B2" s="68" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="C2" s="50" t="n">
         <v>1</v>
@@ -4762,7 +4766,7 @@
       </c>
       <c r="E2" s="69"/>
       <c r="F2" s="78" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="G2" s="54" t="s">
         <v>61</v>
@@ -4774,7 +4778,7 @@
     <row r="3" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="48"/>
       <c r="B3" s="68" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="C3" s="56" t="n">
         <v>1</v>
@@ -4784,7 +4788,7 @@
       </c>
       <c r="E3" s="28"/>
       <c r="F3" s="79" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="G3" s="29" t="s">
         <v>61</v>
@@ -4796,7 +4800,7 @@
     <row r="4" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="48"/>
       <c r="B4" s="68" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="C4" s="56" t="n">
         <v>1</v>
@@ -4806,7 +4810,7 @@
       </c>
       <c r="E4" s="28"/>
       <c r="F4" s="79" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="G4" s="29" t="s">
         <v>61</v>
@@ -4817,10 +4821,10 @@
     </row>
     <row r="5" customFormat="false" ht="63.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="48" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="B5" s="68" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="C5" s="60" t="n">
         <v>2</v>
@@ -4830,7 +4834,7 @@
       </c>
       <c r="E5" s="28"/>
       <c r="F5" s="79" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="G5" s="29" t="s">
         <v>61</v>
@@ -4842,7 +4846,7 @@
     <row r="6" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="48"/>
       <c r="B6" s="68" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="C6" s="60" t="n">
         <v>2</v>
@@ -4852,7 +4856,7 @@
       </c>
       <c r="E6" s="28"/>
       <c r="F6" s="79" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="G6" s="29" t="s">
         <v>61</v>
@@ -4864,7 +4868,7 @@
     <row r="7" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="48"/>
       <c r="B7" s="68" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="C7" s="60" t="n">
         <v>2</v>
@@ -4874,7 +4878,7 @@
       </c>
       <c r="E7" s="28"/>
       <c r="F7" s="79" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="G7" s="29" t="s">
         <v>26</v>
@@ -4886,7 +4890,7 @@
     <row r="8" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="48"/>
       <c r="B8" s="68" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="C8" s="60" t="n">
         <v>2</v>
@@ -4896,7 +4900,7 @@
       </c>
       <c r="E8" s="28"/>
       <c r="F8" s="79" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="G8" s="29" t="s">
         <v>61</v>
@@ -4908,7 +4912,7 @@
     <row r="9" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="48"/>
       <c r="B9" s="68" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="C9" s="93" t="n">
         <v>3</v>
@@ -4918,7 +4922,7 @@
       </c>
       <c r="E9" s="38"/>
       <c r="F9" s="80" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="G9" s="39" t="s">
         <v>61</v>
@@ -5006,10 +5010,10 @@
     </row>
     <row r="2" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="48" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="B2" s="68" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="C2" s="95" t="n">
         <v>3</v>
@@ -5019,25 +5023,25 @@
       </c>
       <c r="E2" s="69"/>
       <c r="F2" s="78" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="G2" s="54" t="s">
         <v>26</v>
       </c>
       <c r="H2" s="54" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="I2" s="54"/>
       <c r="J2" s="55" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="48" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="B3" s="68" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="C3" s="60" t="n">
         <v>2</v>
@@ -5047,13 +5051,13 @@
       </c>
       <c r="E3" s="28"/>
       <c r="F3" s="79" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="G3" s="29" t="s">
         <v>26</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="I3" s="29"/>
       <c r="J3" s="33"/>
@@ -5061,7 +5065,7 @@
     <row r="4" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="48"/>
       <c r="B4" s="68" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="C4" s="60" t="n">
         <v>2</v>
@@ -5071,13 +5075,13 @@
       </c>
       <c r="E4" s="28"/>
       <c r="F4" s="79" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="G4" s="29" t="s">
         <v>26</v>
       </c>
       <c r="H4" s="29" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="I4" s="29"/>
       <c r="J4" s="33"/>
@@ -5085,7 +5089,7 @@
     <row r="5" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="48"/>
       <c r="B5" s="68" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="C5" s="59" t="n">
         <v>3</v>
@@ -5095,13 +5099,13 @@
       </c>
       <c r="E5" s="28"/>
       <c r="F5" s="79" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="G5" s="29" t="s">
         <v>26</v>
       </c>
       <c r="H5" s="29" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="I5" s="29"/>
       <c r="J5" s="33"/>
@@ -5109,7 +5113,7 @@
     <row r="6" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="48"/>
       <c r="B6" s="68" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="C6" s="59" t="n">
         <v>3</v>
@@ -5119,13 +5123,13 @@
       </c>
       <c r="E6" s="28"/>
       <c r="F6" s="79" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="G6" s="29" t="s">
         <v>26</v>
       </c>
       <c r="H6" s="29" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="I6" s="29"/>
       <c r="J6" s="33"/>
@@ -5133,7 +5137,7 @@
     <row r="7" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="48"/>
       <c r="B7" s="68" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="C7" s="59" t="n">
         <v>3</v>
@@ -5143,13 +5147,13 @@
       </c>
       <c r="E7" s="28"/>
       <c r="F7" s="79" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="G7" s="29" t="s">
         <v>26</v>
       </c>
       <c r="H7" s="29" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="I7" s="29"/>
       <c r="J7" s="33"/>
@@ -5157,7 +5161,7 @@
     <row r="8" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="48"/>
       <c r="B8" s="68" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="C8" s="59" t="n">
         <v>3</v>
@@ -5167,23 +5171,23 @@
       </c>
       <c r="E8" s="28"/>
       <c r="F8" s="79" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="G8" s="29" t="s">
         <v>26</v>
       </c>
       <c r="H8" s="29" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="I8" s="29"/>
       <c r="J8" s="33"/>
     </row>
     <row r="9" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="48" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="B9" s="68" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="C9" s="56" t="n">
         <v>1</v>
@@ -5193,7 +5197,7 @@
       </c>
       <c r="E9" s="28"/>
       <c r="F9" s="79" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="G9" s="29" t="s">
         <v>90</v>
@@ -5205,7 +5209,7 @@
     <row r="10" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="48"/>
       <c r="B10" s="68" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="C10" s="56" t="n">
         <v>1</v>
@@ -5215,7 +5219,7 @@
       </c>
       <c r="E10" s="28"/>
       <c r="F10" s="79" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="G10" s="29" t="s">
         <v>26</v>
@@ -5227,7 +5231,7 @@
     <row r="11" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="48"/>
       <c r="B11" s="68" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="C11" s="70" t="n">
         <v>1</v>
@@ -5237,7 +5241,7 @@
       </c>
       <c r="E11" s="38"/>
       <c r="F11" s="80" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="G11" s="39" t="s">
         <v>61</v>
@@ -5274,8 +5278,8 @@
   </sheetPr>
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5325,10 +5329,10 @@
     </row>
     <row r="2" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="48" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="B2" s="68" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="C2" s="50" t="n">
         <v>1</v>
@@ -5338,13 +5342,13 @@
       </c>
       <c r="E2" s="69"/>
       <c r="F2" s="78" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="G2" s="54" t="s">
         <v>26</v>
       </c>
       <c r="H2" s="54" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="I2" s="54"/>
       <c r="J2" s="55"/>
@@ -5352,7 +5356,7 @@
     <row r="3" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="48"/>
       <c r="B3" s="68" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="C3" s="56" t="n">
         <v>1</v>
@@ -5362,7 +5366,7 @@
       </c>
       <c r="E3" s="28"/>
       <c r="F3" s="79" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="G3" s="29" t="s">
         <v>26</v>
@@ -5374,7 +5378,7 @@
     <row r="4" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="48"/>
       <c r="B4" s="68" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="C4" s="56" t="n">
         <v>1</v>
@@ -5384,7 +5388,7 @@
       </c>
       <c r="E4" s="28"/>
       <c r="F4" s="79" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="G4" s="29" t="s">
         <v>26</v>
@@ -5396,7 +5400,7 @@
     <row r="5" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="48"/>
       <c r="B5" s="68" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="C5" s="56" t="n">
         <v>1</v>
@@ -5406,10 +5410,10 @@
       </c>
       <c r="E5" s="28"/>
       <c r="F5" s="79" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="G5" s="29" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
       <c r="H5" s="29"/>
       <c r="I5" s="29"/>
@@ -5418,7 +5422,7 @@
     <row r="6" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="48"/>
       <c r="B6" s="68" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="C6" s="56" t="n">
         <v>1</v>
@@ -5428,7 +5432,7 @@
       </c>
       <c r="E6" s="28"/>
       <c r="F6" s="79" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="G6" s="29" t="s">
         <v>26</v>
@@ -5440,7 +5444,7 @@
     <row r="7" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="48"/>
       <c r="B7" s="68" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="C7" s="60" t="n">
         <v>2</v>
@@ -5450,7 +5454,7 @@
       </c>
       <c r="E7" s="28"/>
       <c r="F7" s="79" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="G7" s="29"/>
       <c r="H7" s="29"/>
@@ -5460,7 +5464,7 @@
     <row r="8" customFormat="false" ht="66.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="48"/>
       <c r="B8" s="68" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="C8" s="60" t="n">
         <v>2</v>
@@ -5470,7 +5474,7 @@
       </c>
       <c r="E8" s="28"/>
       <c r="F8" s="79" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="G8" s="29" t="s">
         <v>90</v>
@@ -5482,7 +5486,7 @@
     <row r="9" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="48"/>
       <c r="B9" s="68" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="C9" s="77" t="n">
         <v>2</v>
@@ -5492,7 +5496,7 @@
       </c>
       <c r="E9" s="38"/>
       <c r="F9" s="80" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="G9" s="39" t="s">
         <v>90</v>
@@ -5579,10 +5583,10 @@
     </row>
     <row r="2" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="48" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="B2" s="68" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="C2" s="50" t="n">
         <v>1</v>
@@ -5592,7 +5596,7 @@
       </c>
       <c r="E2" s="69"/>
       <c r="F2" s="78" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="G2" s="54"/>
       <c r="H2" s="54"/>
@@ -5602,7 +5606,7 @@
     <row r="3" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="48"/>
       <c r="B3" s="68" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="C3" s="60" t="n">
         <v>2</v>
@@ -5612,7 +5616,7 @@
       </c>
       <c r="E3" s="28"/>
       <c r="F3" s="79" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="G3" s="29"/>
       <c r="H3" s="29"/>
@@ -5622,7 +5626,7 @@
     <row r="4" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="48"/>
       <c r="B4" s="68" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="C4" s="60" t="n">
         <v>2</v>
@@ -5632,7 +5636,7 @@
       </c>
       <c r="E4" s="28"/>
       <c r="F4" s="79" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="G4" s="29"/>
       <c r="H4" s="29"/>
@@ -5641,10 +5645,10 @@
     </row>
     <row r="5" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="48" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="B5" s="68" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="C5" s="60" t="n">
         <v>2</v>
@@ -5654,7 +5658,7 @@
       </c>
       <c r="E5" s="28"/>
       <c r="F5" s="79" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="G5" s="29"/>
       <c r="H5" s="29"/>
@@ -5663,10 +5667,10 @@
     </row>
     <row r="6" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="48" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="B6" s="68" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="C6" s="56" t="n">
         <v>1</v>
@@ -5676,7 +5680,7 @@
       </c>
       <c r="E6" s="28"/>
       <c r="F6" s="79" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="G6" s="29"/>
       <c r="H6" s="29"/>
@@ -5686,7 +5690,7 @@
     <row r="7" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="48"/>
       <c r="B7" s="68" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="C7" s="56" t="n">
         <v>1</v>
@@ -5696,7 +5700,7 @@
       </c>
       <c r="E7" s="28"/>
       <c r="F7" s="79" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="G7" s="29"/>
       <c r="H7" s="29"/>
@@ -5706,7 +5710,7 @@
     <row r="8" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="48"/>
       <c r="B8" s="68" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="C8" s="56" t="n">
         <v>1</v>
@@ -5716,7 +5720,7 @@
       </c>
       <c r="E8" s="28"/>
       <c r="F8" s="79" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="G8" s="29"/>
       <c r="H8" s="29"/>
@@ -5726,7 +5730,7 @@
     <row r="9" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="48"/>
       <c r="B9" s="68" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="C9" s="56" t="n">
         <v>1</v>
@@ -5736,7 +5740,7 @@
       </c>
       <c r="E9" s="28"/>
       <c r="F9" s="79" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="G9" s="29"/>
       <c r="H9" s="29"/>
@@ -5746,7 +5750,7 @@
     <row r="10" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="48"/>
       <c r="B10" s="68" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="C10" s="56" t="n">
         <v>1</v>
@@ -5756,7 +5760,7 @@
       </c>
       <c r="E10" s="28"/>
       <c r="F10" s="79" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="G10" s="29"/>
       <c r="H10" s="29"/>
@@ -5766,7 +5770,7 @@
     <row r="11" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="48"/>
       <c r="B11" s="68" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="C11" s="60" t="n">
         <v>2</v>
@@ -5776,7 +5780,7 @@
       </c>
       <c r="E11" s="28"/>
       <c r="F11" s="79" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="G11" s="29"/>
       <c r="H11" s="29"/>
@@ -5785,10 +5789,10 @@
     </row>
     <row r="12" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="48" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="B12" s="68" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="C12" s="56" t="n">
         <v>1</v>
@@ -5798,7 +5802,7 @@
       </c>
       <c r="E12" s="28"/>
       <c r="F12" s="79" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="G12" s="29"/>
       <c r="H12" s="29"/>
@@ -5808,7 +5812,7 @@
     <row r="13" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="48"/>
       <c r="B13" s="68" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="C13" s="56" t="n">
         <v>1</v>
@@ -5818,7 +5822,7 @@
       </c>
       <c r="E13" s="28"/>
       <c r="F13" s="79" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="G13" s="29"/>
       <c r="H13" s="29"/>
@@ -5827,10 +5831,10 @@
     </row>
     <row r="14" customFormat="false" ht="79.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="48" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="B14" s="68" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="C14" s="56" t="n">
         <v>1</v>
@@ -5840,7 +5844,7 @@
       </c>
       <c r="E14" s="28"/>
       <c r="F14" s="79" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="G14" s="29"/>
       <c r="H14" s="29"/>
@@ -5850,7 +5854,7 @@
     <row r="15" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="48"/>
       <c r="B15" s="68" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="C15" s="56" t="n">
         <v>1</v>
@@ -5860,7 +5864,7 @@
       </c>
       <c r="E15" s="28"/>
       <c r="F15" s="79" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="G15" s="29"/>
       <c r="H15" s="29"/>
@@ -5869,10 +5873,10 @@
     </row>
     <row r="16" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="48" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="B16" s="68" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="C16" s="70" t="n">
         <v>1</v>
@@ -5882,7 +5886,7 @@
       </c>
       <c r="E16" s="38"/>
       <c r="F16" s="80" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="G16" s="39"/>
       <c r="H16" s="39"/>
@@ -5920,7 +5924,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5969,10 +5973,10 @@
     </row>
     <row r="2" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="48" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="B2" s="68" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="C2" s="50" t="n">
         <v>1</v>
@@ -5982,11 +5986,11 @@
       </c>
       <c r="E2" s="69"/>
       <c r="F2" s="78" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="G2" s="54"/>
       <c r="H2" s="54" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="I2" s="54"/>
       <c r="J2" s="55"/>
@@ -5994,7 +5998,7 @@
     <row r="3" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="48"/>
       <c r="B3" s="68" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="C3" s="56" t="n">
         <v>1</v>
@@ -6004,7 +6008,7 @@
       </c>
       <c r="E3" s="28"/>
       <c r="F3" s="79" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="G3" s="29" t="s">
         <v>61</v>
@@ -6016,7 +6020,7 @@
     <row r="4" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="48"/>
       <c r="B4" s="68" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="C4" s="56" t="n">
         <v>1</v>
@@ -6026,13 +6030,13 @@
       </c>
       <c r="E4" s="28"/>
       <c r="F4" s="79" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="G4" s="29" t="s">
         <v>26</v>
       </c>
       <c r="H4" s="29" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="I4" s="29"/>
       <c r="J4" s="33"/>
@@ -6040,7 +6044,7 @@
     <row r="5" customFormat="false" ht="132.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="48"/>
       <c r="B5" s="68" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="C5" s="60" t="n">
         <v>2</v>
@@ -6050,23 +6054,23 @@
       </c>
       <c r="E5" s="28"/>
       <c r="F5" s="79" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="G5" s="29" t="s">
         <v>26</v>
       </c>
       <c r="H5" s="31" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="I5" s="29"/>
       <c r="J5" s="33" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="48"/>
       <c r="B6" s="68" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="C6" s="60" t="n">
         <v>2</v>
@@ -6076,23 +6080,23 @@
       </c>
       <c r="E6" s="28"/>
       <c r="F6" s="79" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="G6" s="29" t="s">
         <v>26</v>
       </c>
       <c r="H6" s="29" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="I6" s="29"/>
       <c r="J6" s="33"/>
     </row>
     <row r="7" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="48" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="B7" s="68" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="C7" s="56" t="n">
         <v>1</v>
@@ -6102,13 +6106,13 @@
       </c>
       <c r="E7" s="28"/>
       <c r="F7" s="79" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="G7" s="29" t="s">
         <v>26</v>
       </c>
       <c r="H7" s="29" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="I7" s="29"/>
       <c r="J7" s="33"/>
@@ -6116,7 +6120,7 @@
     <row r="8" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="48"/>
       <c r="B8" s="68" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="C8" s="56" t="n">
         <v>1</v>
@@ -6126,13 +6130,13 @@
       </c>
       <c r="E8" s="28"/>
       <c r="F8" s="79" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="G8" s="29" t="s">
         <v>26</v>
       </c>
       <c r="H8" s="29" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="I8" s="29"/>
       <c r="J8" s="33"/>
@@ -6140,7 +6144,7 @@
     <row r="9" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="48"/>
       <c r="B9" s="68" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="C9" s="56" t="n">
         <v>1</v>
@@ -6150,7 +6154,7 @@
       </c>
       <c r="E9" s="28"/>
       <c r="F9" s="79" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="G9" s="29" t="s">
         <v>61</v>
@@ -6162,7 +6166,7 @@
     <row r="10" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="48"/>
       <c r="B10" s="68" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="C10" s="60" t="n">
         <v>2</v>
@@ -6172,7 +6176,7 @@
       </c>
       <c r="E10" s="28"/>
       <c r="F10" s="79" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="G10" s="29" t="s">
         <v>61</v>
@@ -6184,7 +6188,7 @@
     <row r="11" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="48"/>
       <c r="B11" s="68" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="C11" s="60" t="n">
         <v>2</v>
@@ -6194,21 +6198,21 @@
       </c>
       <c r="E11" s="28"/>
       <c r="F11" s="79" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="G11" s="29" t="s">
         <v>26</v>
       </c>
       <c r="H11" s="29" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="I11" s="29"/>
       <c r="J11" s="33"/>
     </row>
-    <row r="12" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="72.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="48"/>
       <c r="B12" s="68" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="C12" s="60" t="n">
         <v>2</v>
@@ -6218,10 +6222,10 @@
       </c>
       <c r="E12" s="28"/>
       <c r="F12" s="79" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="G12" s="29" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
       <c r="H12" s="29"/>
       <c r="I12" s="29"/>
@@ -6229,10 +6233,10 @@
     </row>
     <row r="13" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="48" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="B13" s="68" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="C13" s="56" t="n">
         <v>1</v>
@@ -6242,13 +6246,13 @@
       </c>
       <c r="E13" s="28"/>
       <c r="F13" s="79" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="G13" s="29" t="s">
         <v>61</v>
       </c>
       <c r="H13" s="29" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="I13" s="29"/>
       <c r="J13" s="33"/>
@@ -6256,7 +6260,7 @@
     <row r="14" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="48"/>
       <c r="B14" s="68" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="C14" s="60" t="n">
         <v>2</v>
@@ -6266,7 +6270,7 @@
       </c>
       <c r="E14" s="28"/>
       <c r="F14" s="79" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="G14" s="29" t="s">
         <v>61</v>
@@ -6277,10 +6281,10 @@
     </row>
     <row r="15" customFormat="false" ht="63.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="48" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="B15" s="68" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="C15" s="60" t="n">
         <v>2</v>
@@ -6290,7 +6294,7 @@
       </c>
       <c r="E15" s="28"/>
       <c r="F15" s="79" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="G15" s="29" t="s">
         <v>61</v>
@@ -6302,7 +6306,7 @@
     <row r="16" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="48"/>
       <c r="B16" s="68" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="C16" s="77" t="n">
         <v>2</v>
@@ -6312,7 +6316,7 @@
       </c>
       <c r="E16" s="38"/>
       <c r="F16" s="80" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="G16" s="39" t="s">
         <v>61</v>
@@ -6351,7 +6355,7 @@
   </sheetPr>
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -6402,10 +6406,10 @@
     </row>
     <row r="2" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="97" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="B2" s="98" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="C2" s="99" t="n">
         <v>2</v>
@@ -6413,23 +6417,23 @@
       <c r="D2" s="100"/>
       <c r="E2" s="100"/>
       <c r="F2" s="101" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="G2" s="102" t="s">
         <v>26</v>
       </c>
       <c r="H2" s="102" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="I2" s="102"/>
       <c r="J2" s="103" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="97"/>
       <c r="B3" s="68" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="C3" s="104" t="n">
         <v>2</v>
@@ -6439,13 +6443,13 @@
       </c>
       <c r="E3" s="105"/>
       <c r="F3" s="106" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="G3" s="107" t="s">
         <v>61</v>
       </c>
       <c r="H3" s="107" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="I3" s="107"/>
       <c r="J3" s="108"/>
@@ -6453,7 +6457,7 @@
     <row r="4" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="97"/>
       <c r="B4" s="68" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="C4" s="104" t="n">
         <v>2</v>
@@ -6463,23 +6467,23 @@
       </c>
       <c r="E4" s="105"/>
       <c r="F4" s="106" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="G4" s="107" t="s">
         <v>26</v>
       </c>
       <c r="H4" s="107" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="I4" s="107"/>
       <c r="J4" s="108" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="97"/>
       <c r="B5" s="68" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="C5" s="104" t="n">
         <v>2</v>
@@ -6487,23 +6491,23 @@
       <c r="D5" s="105"/>
       <c r="E5" s="105"/>
       <c r="F5" s="106" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="G5" s="107" t="s">
         <v>26</v>
       </c>
       <c r="H5" s="107" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="I5" s="107"/>
       <c r="J5" s="108" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="97"/>
       <c r="B6" s="68" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="C6" s="109" t="n">
         <v>3</v>
@@ -6511,25 +6515,25 @@
       <c r="D6" s="105"/>
       <c r="E6" s="105"/>
       <c r="F6" s="106" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="G6" s="107" t="s">
         <v>26</v>
       </c>
       <c r="H6" s="110" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="I6" s="107"/>
       <c r="J6" s="108" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="48" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="B7" s="68" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="C7" s="111" t="n">
         <v>1</v>
@@ -6539,23 +6543,23 @@
       </c>
       <c r="E7" s="105"/>
       <c r="F7" s="106" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="G7" s="107" t="s">
         <v>26</v>
       </c>
       <c r="H7" s="107" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="I7" s="107"/>
       <c r="J7" s="108" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="48"/>
       <c r="B8" s="68" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="C8" s="111" t="n">
         <v>1</v>
@@ -6565,13 +6569,13 @@
       </c>
       <c r="E8" s="105"/>
       <c r="F8" s="106" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="G8" s="107" t="s">
         <v>26</v>
       </c>
       <c r="H8" s="107" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="I8" s="107"/>
       <c r="J8" s="108"/>
@@ -6579,7 +6583,7 @@
     <row r="9" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="48"/>
       <c r="B9" s="68" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="C9" s="111" t="n">
         <v>1</v>
@@ -6589,13 +6593,13 @@
       </c>
       <c r="E9" s="105"/>
       <c r="F9" s="106" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="G9" s="107" t="s">
         <v>26</v>
       </c>
       <c r="H9" s="107" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="I9" s="107"/>
       <c r="J9" s="108"/>
@@ -6603,7 +6607,7 @@
     <row r="10" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="48"/>
       <c r="B10" s="68" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="C10" s="104" t="n">
         <v>2</v>
@@ -6613,21 +6617,21 @@
       </c>
       <c r="E10" s="105"/>
       <c r="F10" s="106" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="G10" s="107"/>
       <c r="H10" s="107" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="I10" s="107"/>
       <c r="J10" s="108" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="48"/>
       <c r="B11" s="68" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="C11" s="104" t="n">
         <v>2</v>
@@ -6635,7 +6639,7 @@
       <c r="D11" s="105"/>
       <c r="E11" s="105"/>
       <c r="F11" s="106" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="G11" s="107" t="s">
         <v>90</v>
@@ -6647,7 +6651,7 @@
     <row r="12" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="48"/>
       <c r="B12" s="68" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="C12" s="104" t="n">
         <v>2</v>
@@ -6657,23 +6661,23 @@
       </c>
       <c r="E12" s="105"/>
       <c r="F12" s="106" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="G12" s="107" t="s">
         <v>26</v>
       </c>
       <c r="H12" s="107" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="I12" s="107"/>
       <c r="J12" s="108"/>
     </row>
     <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="48" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="B13" s="68" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="C13" s="111" t="n">
         <v>1</v>
@@ -6683,7 +6687,7 @@
       </c>
       <c r="E13" s="105"/>
       <c r="F13" s="106" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="G13" s="107" t="s">
         <v>61</v>
@@ -6695,7 +6699,7 @@
     <row r="14" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="48"/>
       <c r="B14" s="68" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="C14" s="111" t="n">
         <v>1</v>
@@ -6705,13 +6709,13 @@
       </c>
       <c r="E14" s="105"/>
       <c r="F14" s="106" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="G14" s="107" t="s">
         <v>26</v>
       </c>
       <c r="H14" s="107" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="I14" s="107"/>
       <c r="J14" s="108"/>
@@ -6719,7 +6723,7 @@
     <row r="15" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="48"/>
       <c r="B15" s="68" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="C15" s="111" t="n">
         <v>1</v>
@@ -6729,23 +6733,23 @@
       </c>
       <c r="E15" s="105"/>
       <c r="F15" s="106" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="G15" s="107" t="s">
         <v>26</v>
       </c>
       <c r="H15" s="107" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="I15" s="107"/>
       <c r="J15" s="108"/>
     </row>
     <row r="16" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="48" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="B16" s="68" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="C16" s="111" t="n">
         <v>1</v>
@@ -6755,23 +6759,23 @@
       </c>
       <c r="E16" s="105"/>
       <c r="F16" s="106" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="G16" s="107" t="s">
         <v>26</v>
       </c>
       <c r="H16" s="107" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="I16" s="107"/>
       <c r="J16" s="108" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="48"/>
       <c r="B17" s="68" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="C17" s="111" t="n">
         <v>1</v>
@@ -6781,13 +6785,13 @@
       </c>
       <c r="E17" s="105"/>
       <c r="F17" s="106" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="G17" s="107" t="s">
         <v>26</v>
       </c>
       <c r="H17" s="107" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="I17" s="107"/>
       <c r="J17" s="108"/>
@@ -6795,7 +6799,7 @@
     <row r="18" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="48"/>
       <c r="B18" s="68" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="C18" s="111" t="n">
         <v>1</v>
@@ -6805,7 +6809,7 @@
       </c>
       <c r="E18" s="105"/>
       <c r="F18" s="106" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="G18" s="107" t="s">
         <v>61</v>
@@ -6817,7 +6821,7 @@
     <row r="19" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="48"/>
       <c r="B19" s="68" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="C19" s="111" t="n">
         <v>1</v>
@@ -6827,23 +6831,23 @@
       </c>
       <c r="E19" s="105"/>
       <c r="F19" s="106" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="G19" s="107" t="s">
         <v>26</v>
       </c>
       <c r="H19" s="107" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="I19" s="107"/>
       <c r="J19" s="108" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="48"/>
       <c r="B20" s="68" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="C20" s="111" t="n">
         <v>1</v>
@@ -6853,13 +6857,13 @@
       </c>
       <c r="E20" s="105"/>
       <c r="F20" s="106" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="G20" s="107" t="s">
         <v>26</v>
       </c>
       <c r="H20" s="107" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="I20" s="107"/>
       <c r="J20" s="108"/>
@@ -6867,7 +6871,7 @@
     <row r="21" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="48"/>
       <c r="B21" s="68" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="C21" s="111" t="n">
         <v>1</v>
@@ -6877,13 +6881,13 @@
       </c>
       <c r="E21" s="105"/>
       <c r="F21" s="106" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="G21" s="107" t="s">
         <v>26</v>
       </c>
       <c r="H21" s="107" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="I21" s="107"/>
       <c r="J21" s="108"/>
@@ -6891,7 +6895,7 @@
     <row r="22" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="48"/>
       <c r="B22" s="68" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="C22" s="111" t="n">
         <v>1</v>
@@ -6901,7 +6905,7 @@
       </c>
       <c r="E22" s="105"/>
       <c r="F22" s="106" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="G22" s="107" t="s">
         <v>61</v>
@@ -6912,10 +6916,10 @@
     </row>
     <row r="23" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="48" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="B23" s="68" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="C23" s="111" t="n">
         <v>1</v>
@@ -6925,13 +6929,13 @@
       </c>
       <c r="E23" s="105"/>
       <c r="F23" s="106" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="G23" s="107" t="s">
         <v>26</v>
       </c>
       <c r="H23" s="112" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="I23" s="107"/>
       <c r="J23" s="108"/>
@@ -6939,7 +6943,7 @@
     <row r="24" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="48"/>
       <c r="B24" s="68" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="C24" s="111" t="n">
         <v>1</v>
@@ -6949,13 +6953,13 @@
       </c>
       <c r="E24" s="105"/>
       <c r="F24" s="106" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="G24" s="107" t="s">
         <v>26</v>
       </c>
       <c r="H24" s="107" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="I24" s="107"/>
       <c r="J24" s="108"/>
@@ -6963,7 +6967,7 @@
     <row r="25" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="48"/>
       <c r="B25" s="68" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="C25" s="111" t="n">
         <v>1</v>
@@ -6973,13 +6977,13 @@
       </c>
       <c r="E25" s="105"/>
       <c r="F25" s="106" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="G25" s="107" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="H25" s="107" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="I25" s="107"/>
       <c r="J25" s="108"/>
@@ -6987,7 +6991,7 @@
     <row r="26" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="48"/>
       <c r="B26" s="68" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="C26" s="113" t="n">
         <v>2</v>
@@ -6997,13 +7001,13 @@
       </c>
       <c r="E26" s="114"/>
       <c r="F26" s="115" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="G26" s="116" t="s">
         <v>26</v>
       </c>
       <c r="H26" s="116" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="I26" s="116"/>
       <c r="J26" s="117"/>
@@ -12126,8 +12130,8 @@
   </sheetPr>
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12281,7 +12285,7 @@
         <v>533</v>
       </c>
       <c r="G6" s="29" t="s">
-        <v>90</v>
+        <v>26</v>
       </c>
       <c r="H6" s="29"/>
       <c r="I6" s="29"/>
@@ -12401,7 +12405,7 @@
       <c r="I11" s="29"/>
       <c r="J11" s="33"/>
     </row>
-    <row r="12" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="60.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="48"/>
       <c r="B12" s="68" t="s">
         <v>546</v>
@@ -12417,16 +12421,18 @@
         <v>547</v>
       </c>
       <c r="G12" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="H12" s="29"/>
+        <v>26</v>
+      </c>
+      <c r="H12" s="31" t="s">
+        <v>548</v>
+      </c>
       <c r="I12" s="29"/>
       <c r="J12" s="33"/>
     </row>
     <row r="13" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="48"/>
       <c r="B13" s="68" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="C13" s="56" t="n">
         <v>1</v>
@@ -12436,7 +12442,7 @@
       </c>
       <c r="E13" s="28"/>
       <c r="F13" s="79" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="G13" s="29" t="s">
         <v>90</v>
@@ -12448,7 +12454,7 @@
     <row r="14" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="48"/>
       <c r="B14" s="68" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C14" s="56" t="n">
         <v>1</v>
@@ -12458,7 +12464,7 @@
       </c>
       <c r="E14" s="28"/>
       <c r="F14" s="79" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="G14" s="29" t="s">
         <v>26</v>
@@ -12470,7 +12476,7 @@
     <row r="15" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="48"/>
       <c r="B15" s="68" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="C15" s="60" t="n">
         <v>2</v>
@@ -12480,7 +12486,7 @@
       </c>
       <c r="E15" s="28"/>
       <c r="F15" s="79" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="G15" s="29" t="s">
         <v>90</v>
@@ -12492,7 +12498,7 @@
     <row r="16" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="48"/>
       <c r="B16" s="68" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="C16" s="60" t="n">
         <v>2</v>
@@ -12502,7 +12508,7 @@
       </c>
       <c r="E16" s="28"/>
       <c r="F16" s="79" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="G16" s="29" t="s">
         <v>90</v>
@@ -12514,7 +12520,7 @@
     <row r="17" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="48"/>
       <c r="B17" s="68" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="C17" s="60" t="n">
         <v>2</v>
@@ -12524,7 +12530,7 @@
       </c>
       <c r="E17" s="28"/>
       <c r="F17" s="79" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="G17" s="29" t="s">
         <v>26</v>
@@ -12536,7 +12542,7 @@
     <row r="18" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="48"/>
       <c r="B18" s="68" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="C18" s="77" t="n">
         <v>2</v>
@@ -12546,7 +12552,7 @@
       </c>
       <c r="E18" s="38"/>
       <c r="F18" s="80" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="G18" s="39" t="s">
         <v>61</v>

</xml_diff>

<commit_message>
#1 [feat]: set password max length to 128 characters
</commit_message>
<xml_diff>
--- a/Deliverables/v4-ASVS-checklist-en.xlsx
+++ b/Deliverables/v4-ASVS-checklist-en.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodri\OneDrive\Documents\Mestrado\2Semestre\SISMD\PL3\desofs2024_m1b_2\Deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD1061F-A45D-46D3-88C3-560BA37A4876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4261ED-92F6-4153-B2E6-E0E771B15060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3826,7 +3826,7 @@
                   <c:v>84.848484848484844</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>62.857142857142854</c:v>
+                  <c:v>65.714285714285708</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>71.428571428571431</c:v>
@@ -3865,7 +3865,7 @@
                   <c:v>85.714285714285708</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>68.518518518518519</c:v>
+                  <c:v>68.981481481481481</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4314,7 +4314,7 @@
       </c>
       <c r="B3" s="9">
         <f>COUNTIF(Authentication!G2:G58,"Valid")</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C3" s="10">
         <f>COUNTIF(Authentication!G2:G58,"&lt;&gt;Not Applicable")</f>
@@ -4322,7 +4322,7 @@
       </c>
       <c r="D3" s="11">
         <f t="shared" si="0"/>
-        <v>62.857142857142854</v>
+        <v>65.714285714285708</v>
       </c>
       <c r="E3" s="12"/>
     </row>
@@ -4549,7 +4549,7 @@
       </c>
       <c r="B16" s="9">
         <f>SUM(B2:B15)</f>
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C16" s="10">
         <f>SUM(C2:C15)</f>
@@ -4557,7 +4557,7 @@
       </c>
       <c r="D16" s="11">
         <f t="shared" si="0"/>
-        <v>68.518518518518519</v>
+        <v>68.981481481481481</v>
       </c>
       <c r="E16" s="12"/>
     </row>
@@ -8032,17 +8032,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A23:A26"/>
     <mergeCell ref="A40:A45"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="A29:A30"/>
     <mergeCell ref="A31:A32"/>
     <mergeCell ref="A34:A36"/>
     <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A23:A26"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="G2:G45" xr:uid="{00000000-0002-0000-0100-000000000000}">
@@ -8064,7 +8064,7 @@
   <dimension ref="A1:AMJ58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -8157,7 +8157,7 @@
         <v>190</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>90</v>
+        <v>26</v>
       </c>
       <c r="H3" s="30"/>
       <c r="I3" s="30"/>
@@ -9499,16 +9499,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="A39:A44"/>
+    <mergeCell ref="A45:A51"/>
+    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="A55:A58"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="A14:A20"/>
     <mergeCell ref="A21:A23"/>
     <mergeCell ref="A24:A28"/>
     <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="A39:A44"/>
-    <mergeCell ref="A45:A51"/>
-    <mergeCell ref="A52:A54"/>
-    <mergeCell ref="A55:A58"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="G2:G58" xr:uid="{00000000-0002-0000-0200-000000000000}">

</xml_diff>

<commit_message>
#1 [feat]: password strength meter
</commit_message>
<xml_diff>
--- a/Deliverables/v4-ASVS-checklist-en.xlsx
+++ b/Deliverables/v4-ASVS-checklist-en.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodri\OneDrive\Documents\Mestrado\2Semestre\SISMD\PL3\desofs2024_m1b_2\Deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4261ED-92F6-4153-B2E6-E0E771B15060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9B7D6F-1B48-4BD0-978B-59575873C9BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3826,7 +3826,7 @@
                   <c:v>84.848484848484844</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>65.714285714285708</c:v>
+                  <c:v>68.571428571428569</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>71.428571428571431</c:v>
@@ -3865,7 +3865,7 @@
                   <c:v>85.714285714285708</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>68.981481481481481</c:v>
+                  <c:v>69.444444444444443</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4314,7 +4314,7 @@
       </c>
       <c r="B3" s="9">
         <f>COUNTIF(Authentication!G2:G58,"Valid")</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C3" s="10">
         <f>COUNTIF(Authentication!G2:G58,"&lt;&gt;Not Applicable")</f>
@@ -4322,7 +4322,7 @@
       </c>
       <c r="D3" s="11">
         <f t="shared" si="0"/>
-        <v>65.714285714285708</v>
+        <v>68.571428571428569</v>
       </c>
       <c r="E3" s="12"/>
     </row>
@@ -4549,7 +4549,7 @@
       </c>
       <c r="B16" s="9">
         <f>SUM(B2:B15)</f>
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C16" s="10">
         <f>SUM(C2:C15)</f>
@@ -4557,7 +4557,7 @@
       </c>
       <c r="D16" s="11">
         <f t="shared" si="0"/>
-        <v>68.981481481481481</v>
+        <v>69.444444444444443</v>
       </c>
       <c r="E16" s="12"/>
     </row>
@@ -8064,7 +8064,7 @@
   <dimension ref="A1:AMJ58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -8301,7 +8301,7 @@
         <v>202</v>
       </c>
       <c r="G9" s="30" t="s">
-        <v>90</v>
+        <v>26</v>
       </c>
       <c r="H9" s="30"/>
       <c r="I9" s="30"/>

</xml_diff>

<commit_message>
#1 [feat]: password truncation
</commit_message>
<xml_diff>
--- a/Deliverables/v4-ASVS-checklist-en.xlsx
+++ b/Deliverables/v4-ASVS-checklist-en.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodri\OneDrive\Documents\Mestrado\2Semestre\SISMD\PL3\desofs2024_m1b_2\Deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9B7D6F-1B48-4BD0-978B-59575873C9BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9E51F53-80E8-403D-929D-3082E6660EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3826,7 +3826,7 @@
                   <c:v>84.848484848484844</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>68.571428571428569</c:v>
+                  <c:v>71.428571428571431</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>71.428571428571431</c:v>
@@ -3865,7 +3865,7 @@
                   <c:v>85.714285714285708</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>69.444444444444443</c:v>
+                  <c:v>69.907407407407405</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4314,7 +4314,7 @@
       </c>
       <c r="B3" s="9">
         <f>COUNTIF(Authentication!G2:G58,"Valid")</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C3" s="10">
         <f>COUNTIF(Authentication!G2:G58,"&lt;&gt;Not Applicable")</f>
@@ -4322,7 +4322,7 @@
       </c>
       <c r="D3" s="11">
         <f t="shared" si="0"/>
-        <v>68.571428571428569</v>
+        <v>71.428571428571431</v>
       </c>
       <c r="E3" s="12"/>
     </row>
@@ -4549,7 +4549,7 @@
       </c>
       <c r="B16" s="9">
         <f>SUM(B2:B15)</f>
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C16" s="10">
         <f>SUM(C2:C15)</f>
@@ -4557,7 +4557,7 @@
       </c>
       <c r="D16" s="11">
         <f t="shared" si="0"/>
-        <v>69.444444444444443</v>
+        <v>69.907407407407405</v>
       </c>
       <c r="E16" s="12"/>
     </row>
@@ -8032,17 +8032,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A23:A26"/>
     <mergeCell ref="A40:A45"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="A29:A30"/>
     <mergeCell ref="A31:A32"/>
     <mergeCell ref="A34:A36"/>
     <mergeCell ref="A37:A38"/>
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A23:A26"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="G2:G45" xr:uid="{00000000-0002-0000-0100-000000000000}">
@@ -8064,7 +8064,7 @@
   <dimension ref="A1:AMJ58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -8181,7 +8181,7 @@
         <v>192</v>
       </c>
       <c r="G4" s="30" t="s">
-        <v>90</v>
+        <v>26</v>
       </c>
       <c r="H4" s="30"/>
       <c r="I4" s="30"/>
@@ -9499,16 +9499,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="A14:A20"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="A29:A35"/>
     <mergeCell ref="A36:A38"/>
     <mergeCell ref="A39:A44"/>
     <mergeCell ref="A45:A51"/>
     <mergeCell ref="A52:A54"/>
     <mergeCell ref="A55:A58"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="A14:A20"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A24:A28"/>
-    <mergeCell ref="A29:A35"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="G2:G58" xr:uid="{00000000-0002-0000-0200-000000000000}">

</xml_diff>

<commit_message>
#1 [feat]: printable Unicode character
</commit_message>
<xml_diff>
--- a/Deliverables/v4-ASVS-checklist-en.xlsx
+++ b/Deliverables/v4-ASVS-checklist-en.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodri\OneDrive\Documents\Mestrado\2Semestre\SISMD\PL3\desofs2024_m1b_2\Deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9E51F53-80E8-403D-929D-3082E6660EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E59FC9A0-4826-4C2C-80C1-FF4359FAE1D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3826,7 +3826,7 @@
                   <c:v>84.848484848484844</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>71.428571428571431</c:v>
+                  <c:v>74.285714285714292</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>71.428571428571431</c:v>
@@ -3865,7 +3865,7 @@
                   <c:v>85.714285714285708</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>69.907407407407405</c:v>
+                  <c:v>70.370370370370367</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4314,7 +4314,7 @@
       </c>
       <c r="B3" s="9">
         <f>COUNTIF(Authentication!G2:G58,"Valid")</f>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C3" s="10">
         <f>COUNTIF(Authentication!G2:G58,"&lt;&gt;Not Applicable")</f>
@@ -4322,7 +4322,7 @@
       </c>
       <c r="D3" s="11">
         <f t="shared" si="0"/>
-        <v>71.428571428571431</v>
+        <v>74.285714285714292</v>
       </c>
       <c r="E3" s="12"/>
     </row>
@@ -4549,7 +4549,7 @@
       </c>
       <c r="B16" s="9">
         <f>SUM(B2:B15)</f>
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C16" s="10">
         <f>SUM(C2:C15)</f>
@@ -4557,7 +4557,7 @@
       </c>
       <c r="D16" s="11">
         <f t="shared" si="0"/>
-        <v>69.907407407407405</v>
+        <v>70.370370370370367</v>
       </c>
       <c r="E16" s="12"/>
     </row>
@@ -8032,17 +8032,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A23:A26"/>
     <mergeCell ref="A40:A45"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="A29:A30"/>
     <mergeCell ref="A31:A32"/>
     <mergeCell ref="A34:A36"/>
     <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A23:A26"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="G2:G45" xr:uid="{00000000-0002-0000-0100-000000000000}">
@@ -8064,7 +8064,7 @@
   <dimension ref="A1:AMJ58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -8205,7 +8205,7 @@
         <v>194</v>
       </c>
       <c r="G5" s="30" t="s">
-        <v>90</v>
+        <v>26</v>
       </c>
       <c r="H5" s="30"/>
       <c r="I5" s="30"/>
@@ -9499,16 +9499,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="A39:A44"/>
+    <mergeCell ref="A45:A51"/>
+    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="A55:A58"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="A14:A20"/>
     <mergeCell ref="A21:A23"/>
     <mergeCell ref="A24:A28"/>
     <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="A39:A44"/>
-    <mergeCell ref="A45:A51"/>
-    <mergeCell ref="A52:A54"/>
-    <mergeCell ref="A55:A58"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="G2:G58" xr:uid="{00000000-0002-0000-0200-000000000000}">

</xml_diff>

<commit_message>
#1 feat : choose to either temporarily view the entire masked password
</commit_message>
<xml_diff>
--- a/Deliverables/v4-ASVS-checklist-en.xlsx
+++ b/Deliverables/v4-ASVS-checklist-en.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodri\OneDrive\Documents\Mestrado\2Semestre\SISMD\PL3\desofs2024_m1b_2\Deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E59FC9A0-4826-4C2C-80C1-FF4359FAE1D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA3EF4E4-A8C9-43DD-A1BE-5A36094CA685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3826,7 +3826,7 @@
                   <c:v>84.848484848484844</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>74.285714285714292</c:v>
+                  <c:v>77.142857142857153</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>71.428571428571431</c:v>
@@ -3865,7 +3865,7 @@
                   <c:v>85.714285714285708</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>70.370370370370367</c:v>
+                  <c:v>70.833333333333343</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4314,7 +4314,7 @@
       </c>
       <c r="B3" s="9">
         <f>COUNTIF(Authentication!G2:G58,"Valid")</f>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C3" s="10">
         <f>COUNTIF(Authentication!G2:G58,"&lt;&gt;Not Applicable")</f>
@@ -4322,7 +4322,7 @@
       </c>
       <c r="D3" s="11">
         <f t="shared" si="0"/>
-        <v>74.285714285714292</v>
+        <v>77.142857142857153</v>
       </c>
       <c r="E3" s="12"/>
     </row>
@@ -4549,7 +4549,7 @@
       </c>
       <c r="B16" s="9">
         <f>SUM(B2:B15)</f>
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C16" s="10">
         <f>SUM(C2:C15)</f>
@@ -4557,7 +4557,7 @@
       </c>
       <c r="D16" s="11">
         <f t="shared" si="0"/>
-        <v>70.370370370370367</v>
+        <v>70.833333333333343</v>
       </c>
       <c r="E16" s="12"/>
     </row>
@@ -8063,8 +8063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMJ58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="65" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -8397,7 +8397,7 @@
         <v>210</v>
       </c>
       <c r="G13" s="30" t="s">
-        <v>90</v>
+        <v>26</v>
       </c>
       <c r="H13" s="30"/>
       <c r="I13" s="30"/>

</xml_diff>

<commit_message>
#1 feat :  users can change their password and  password change functionality requires the user's current and new password.
</commit_message>
<xml_diff>
--- a/Deliverables/v4-ASVS-checklist-en.xlsx
+++ b/Deliverables/v4-ASVS-checklist-en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodri\OneDrive\Documents\Mestrado\2Semestre\SISMD\PL3\desofs2024_m1b_2\Deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA3EF4E4-A8C9-43DD-A1BE-5A36094CA685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B47602F-3567-4A8C-9406-79927F20EC6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ASVS Results" sheetId="1" r:id="rId1"/>
@@ -3826,7 +3826,7 @@
                   <c:v>84.848484848484844</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>77.142857142857153</c:v>
+                  <c:v>85.294117647058826</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>71.428571428571431</c:v>
@@ -3865,7 +3865,7 @@
                   <c:v>85.714285714285708</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>70.833333333333343</c:v>
+                  <c:v>72.093023255813947</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4259,8 +4259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ16"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -4314,15 +4314,15 @@
       </c>
       <c r="B3" s="9">
         <f>COUNTIF(Authentication!G2:G58,"Valid")</f>
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C3" s="10">
         <f>COUNTIF(Authentication!G2:G58,"&lt;&gt;Not Applicable")</f>
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" s="11">
         <f t="shared" si="0"/>
-        <v>77.142857142857153</v>
+        <v>85.294117647058826</v>
       </c>
       <c r="E3" s="12"/>
     </row>
@@ -4549,15 +4549,15 @@
       </c>
       <c r="B16" s="9">
         <f>SUM(B2:B15)</f>
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C16" s="10">
         <f>SUM(C2:C15)</f>
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D16" s="11">
         <f t="shared" si="0"/>
-        <v>70.833333333333343</v>
+        <v>72.093023255813947</v>
       </c>
       <c r="E16" s="12"/>
     </row>
@@ -6998,7 +6998,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="27" customFormat="1" ht="140.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" s="27" customFormat="1" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A4" s="116"/>
       <c r="B4" s="20" t="s">
         <v>40</v>
@@ -8063,8 +8063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMJ58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="65" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView topLeftCell="A7" zoomScale="65" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -8229,7 +8229,7 @@
         <v>196</v>
       </c>
       <c r="G6" s="30" t="s">
-        <v>90</v>
+        <v>26</v>
       </c>
       <c r="H6" s="30"/>
       <c r="I6" s="30"/>
@@ -8253,7 +8253,7 @@
         <v>198</v>
       </c>
       <c r="G7" s="30" t="s">
-        <v>90</v>
+        <v>26</v>
       </c>
       <c r="H7" s="30"/>
       <c r="I7" s="30"/>
@@ -8277,7 +8277,7 @@
         <v>200</v>
       </c>
       <c r="G8" s="30" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
       <c r="H8" s="30"/>
       <c r="I8" s="30"/>
@@ -9895,7 +9895,7 @@
       <c r="I14" s="30"/>
       <c r="J14" s="34"/>
     </row>
-    <row r="15" spans="1:10" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="78" x14ac:dyDescent="0.3">
       <c r="A15" s="117"/>
       <c r="B15" s="68" t="s">
         <v>360</v>
@@ -11053,7 +11053,7 @@
       <c r="I28" s="30"/>
       <c r="J28" s="34"/>
     </row>
-    <row r="29" spans="1:10" ht="78" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A29" s="117"/>
       <c r="B29" s="68" t="s">
         <v>455</v>

</xml_diff>

<commit_message>
doc: svss updated #4
</commit_message>
<xml_diff>
--- a/Deliverables/v4-ASVS-checklist-en.xlsx
+++ b/Deliverables/v4-ASVS-checklist-en.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodri\OneDrive\Documents\Mestrado\2Semestre\SISMD\PL3\desofs2024_m1b_2\Deliverables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dbeba1083b062d73/Ambiente de Trabalho/Desofs/desofs2024_m1b_2/Deliverables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A4C5237-F738-468E-9773-D0E0FC29FDD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{7A4C5237-F738-468E-9773-D0E0FC29FDD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66BA9101-0D05-4B12-AC17-A33CC0427A35}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" firstSheet="10" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ASVS Results" sheetId="1" r:id="rId1"/>
@@ -29,19 +29,8 @@
     <sheet name="API and Web Service" sheetId="14" r:id="rId14"/>
     <sheet name="Configuration" sheetId="15" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -2458,33 +2447,6 @@
     <t>Indo a \desofs_svelte_front_end\src\lib\scripts.ts , é possível verificar que a aplicação envia o bearer token para o header e não é fornecido pelo utilizador</t>
   </si>
   <si>
-    <t>Iremos implementar um mecanismo de verificação da extensão do ficheiro</t>
-  </si>
-  <si>
-    <t>Iremos implementar um mecanismo que garanta que os ficheiros utilizem o mesmo esquema de codificação UTF-8, e utilizaremos o Apache Tika para detetar o tipo de ficheiro.</t>
-  </si>
-  <si>
-    <t>Através do Springboot iremos limitar o tamanho máximo dos ficheiros, tal como no frontend</t>
-  </si>
-  <si>
-    <t>Para garantir o tipo de ficheiro utilizaremos o Apache Tika</t>
-  </si>
-  <si>
-    <t>Iremos salvar um ficheiro com um nome gerado por nós, de forma a prevenir este tipos de ataques</t>
-  </si>
-  <si>
-    <t>Iremos utilizar mecanismos para permitir apenas ficheiros pdf como o Apache Tika e validações de frontend</t>
-  </si>
-  <si>
-    <t>Iremos verificar o tipo MIME do ficheiro, tal como sanitizar os inputs para prevenir estes problemas</t>
-  </si>
-  <si>
-    <t>Para tal, iremos armaenar os ficheiros num diretório escolhido por nós, com restrição de permissões</t>
-  </si>
-  <si>
-    <t>Optaremos por ignorar o nome do ficheiro, alterando para outro de forma a prevenir ataques</t>
-  </si>
-  <si>
     <t>Springboot e Sveltekit</t>
   </si>
   <si>
@@ -2531,6 +2493,33 @@
   </si>
   <si>
     <t>A funcionalidade foi implementada no frontend, em que o utilizador possui um botão para alterar a forma como visualiza a palavra-passe</t>
+  </si>
+  <si>
+    <t>Através da biblioteca Apache Tika, verificou-se que os ficheiros enviados e recebidos apresentavam o encoding previsto</t>
+  </si>
+  <si>
+    <t>Limitou-se o tamanho dos ficheiros enviados por parte do administrador e gestor de ficheiros.</t>
+  </si>
+  <si>
+    <t>Limitou-se o envio de ficheiros de 1 ficheiro por receita, além de limitar-mos o tamanho máximo do mesmo.</t>
+  </si>
+  <si>
+    <t>Validou-se que os ficheiros eram apenas do tipo pdf através do Apache Tika.</t>
+  </si>
+  <si>
+    <t>Ignorou-se o nome do ficheiro gerando-se um nome por nós, de forma a prevenir este tipo de ataques.</t>
+  </si>
+  <si>
+    <t>Os ficheiros são armazenados numa pasta escolhida por nós denominada "Recipes".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Através do Apache Tika e validações do java, validamos que os ficheiros enviados são apenas do tipo .pdf, negando qualquer operação com outro tipo de extensão de ficheiro. </t>
+  </si>
+  <si>
+    <t>Verificou-se o tipo MIME do ficheiro, tal como sanitizamos os inputs para prevenir estes problemas</t>
+  </si>
+  <si>
+    <t>Ignorou-se o nome do ficheiro gerando-se um nome por nós e colocou-se e garantiu-se que o content-type é plain text e que o content-disposition apresenta um nome fixo</t>
   </si>
 </sst>
 </file>
@@ -3867,7 +3856,7 @@
                     <a:latin typeface="Calibri"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="pt-PT"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -3941,7 +3930,7 @@
             <c:numRef>
               <c:f>'ASVS Results'!$D$2:$D$16</c:f>
               <c:numCache>
-                <c:formatCode>#,##0.00,_€;\-#,##0.00,_€</c:formatCode>
+                <c:formatCode>#\ ##0.00\ _€;\-#\ ##0.00\ _€</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>84.848484848484844</c:v>
@@ -3977,16 +3966,16 @@
                   <c:v>57.142857142857139</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>85.714285714285708</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>90.476190476190482</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>77.184466019417471</c:v>
+                  <c:v>82.524271844660191</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4046,7 +4035,7 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="53282369"/>
@@ -4097,7 +4086,7 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="44868616"/>
@@ -4134,7 +4123,7 @@
               <a:latin typeface="Calibri"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4380,7 +4369,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ16"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A27" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
@@ -4616,7 +4605,7 @@
       </c>
       <c r="B13" s="9">
         <f>COUNTIF('Files and Resources'!G2:G16,"Valid")</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C13" s="10">
         <f>COUNTIF('Files and Resources'!G2:G16,"&lt;&gt;Not Applicable")</f>
@@ -4624,7 +4613,7 @@
       </c>
       <c r="D13" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E13" s="12"/>
     </row>
@@ -4634,7 +4623,7 @@
       </c>
       <c r="B14" s="9">
         <f>COUNTIF('API and Web Service'!G2:G16,"Valid")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C14" s="10">
         <f>COUNTIF('API and Web Service'!G2:G16,"&lt;&gt;Not Applicable")</f>
@@ -4642,7 +4631,7 @@
       </c>
       <c r="D14" s="11">
         <f t="shared" si="0"/>
-        <v>85.714285714285708</v>
+        <v>100</v>
       </c>
       <c r="E14" s="12"/>
     </row>
@@ -4670,7 +4659,7 @@
       </c>
       <c r="B16" s="9">
         <f>SUM(B2:B15)</f>
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="C16" s="10">
         <f>SUM(C2:C15)</f>
@@ -4678,7 +4667,7 @@
       </c>
       <c r="D16" s="11">
         <f t="shared" si="0"/>
-        <v>77.184466019417471</v>
+        <v>82.524271844660191</v>
       </c>
       <c r="E16" s="12"/>
     </row>
@@ -4950,7 +4939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AMJ11"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -5265,7 +5254,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:AMJ9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
@@ -5516,7 +5505,7 @@
   <dimension ref="A1:AMJ16"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -5564,7 +5553,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="63" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="124" t="s">
         <v>628</v>
       </c>
@@ -5582,10 +5571,10 @@
         <v>630</v>
       </c>
       <c r="G2" s="54" t="s">
-        <v>90</v>
+        <v>26</v>
       </c>
       <c r="H2" s="117" t="s">
-        <v>792</v>
+        <v>807</v>
       </c>
       <c r="I2" s="54"/>
       <c r="J2" s="55"/>
@@ -5612,7 +5601,7 @@
       <c r="I3" s="30"/>
       <c r="J3" s="34"/>
     </row>
-    <row r="4" spans="1:10" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="63" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="124"/>
       <c r="B4" s="68" t="s">
         <v>633</v>
@@ -5628,15 +5617,15 @@
         <v>634</v>
       </c>
       <c r="G4" s="30" t="s">
-        <v>90</v>
+        <v>26</v>
       </c>
       <c r="H4" s="32" t="s">
-        <v>790</v>
+        <v>808</v>
       </c>
       <c r="I4" s="30"/>
       <c r="J4" s="34"/>
     </row>
-    <row r="5" spans="1:10" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>635</v>
       </c>
@@ -5654,10 +5643,10 @@
         <v>637</v>
       </c>
       <c r="G5" s="30" t="s">
-        <v>90</v>
+        <v>26</v>
       </c>
       <c r="H5" s="32" t="s">
-        <v>793</v>
+        <v>809</v>
       </c>
       <c r="I5" s="30"/>
       <c r="J5" s="34"/>
@@ -5680,10 +5669,10 @@
         <v>640</v>
       </c>
       <c r="G6" s="30" t="s">
-        <v>90</v>
+        <v>26</v>
       </c>
       <c r="H6" s="32" t="s">
-        <v>794</v>
+        <v>810</v>
       </c>
       <c r="I6" s="30"/>
       <c r="J6" s="34"/>
@@ -5704,10 +5693,10 @@
         <v>642</v>
       </c>
       <c r="G7" s="30" t="s">
-        <v>90</v>
+        <v>26</v>
       </c>
       <c r="H7" s="32" t="s">
-        <v>794</v>
+        <v>810</v>
       </c>
       <c r="I7" s="30"/>
       <c r="J7" s="34"/>
@@ -5728,15 +5717,15 @@
         <v>644</v>
       </c>
       <c r="G8" s="30" t="s">
-        <v>90</v>
+        <v>26</v>
       </c>
       <c r="H8" s="32" t="s">
-        <v>794</v>
+        <v>810</v>
       </c>
       <c r="I8" s="30"/>
       <c r="J8" s="34"/>
     </row>
-    <row r="9" spans="1:10" ht="63" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="94.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="124"/>
       <c r="B9" s="68" t="s">
         <v>645</v>
@@ -5752,10 +5741,10 @@
         <v>646</v>
       </c>
       <c r="G9" s="30" t="s">
-        <v>90</v>
+        <v>26</v>
       </c>
       <c r="H9" s="120" t="s">
-        <v>798</v>
+        <v>814</v>
       </c>
       <c r="I9" s="30"/>
       <c r="J9" s="34"/>
@@ -5798,15 +5787,15 @@
         <v>650</v>
       </c>
       <c r="G11" s="30" t="s">
-        <v>90</v>
+        <v>26</v>
       </c>
       <c r="H11" s="32" t="s">
-        <v>796</v>
+        <v>813</v>
       </c>
       <c r="I11" s="30"/>
       <c r="J11" s="34"/>
     </row>
-    <row r="12" spans="1:10" ht="63" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="124" t="s">
         <v>651</v>
       </c>
@@ -5824,10 +5813,10 @@
         <v>653</v>
       </c>
       <c r="G12" s="30" t="s">
-        <v>90</v>
+        <v>26</v>
       </c>
       <c r="H12" s="32" t="s">
-        <v>797</v>
+        <v>811</v>
       </c>
       <c r="I12" s="30"/>
       <c r="J12" s="34"/>
@@ -5854,7 +5843,7 @@
       <c r="I13" s="30"/>
       <c r="J13" s="34"/>
     </row>
-    <row r="14" spans="1:10" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="94.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="124" t="s">
         <v>656</v>
       </c>
@@ -5872,10 +5861,10 @@
         <v>658</v>
       </c>
       <c r="G14" s="30" t="s">
-        <v>90</v>
+        <v>26</v>
       </c>
       <c r="H14" s="119" t="s">
-        <v>795</v>
+        <v>812</v>
       </c>
       <c r="I14" s="30"/>
       <c r="J14" s="34"/>
@@ -5952,8 +5941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:AMJ16"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -6000,7 +5989,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A2" s="124" t="s">
         <v>664</v>
       </c>
@@ -6018,10 +6007,10 @@
         <v>666</v>
       </c>
       <c r="G2" s="54" t="s">
-        <v>90</v>
+        <v>26</v>
       </c>
       <c r="H2" s="118" t="s">
-        <v>791</v>
+        <v>806</v>
       </c>
       <c r="I2" s="54"/>
       <c r="J2" s="55"/>
@@ -6382,8 +6371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:AMJ26"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -8207,17 +8196,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A23:A26"/>
     <mergeCell ref="A40:A45"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="A29:A30"/>
     <mergeCell ref="A31:A32"/>
     <mergeCell ref="A34:A36"/>
     <mergeCell ref="A37:A38"/>
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A23:A26"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="G2:G45" xr:uid="{00000000-0002-0000-0100-000000000000}">
@@ -8238,7 +8227,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMJ58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="81" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
@@ -8311,11 +8300,11 @@
         <v>26</v>
       </c>
       <c r="H2" s="54" t="s">
-        <v>805</v>
+        <v>796</v>
       </c>
       <c r="I2" s="54"/>
       <c r="J2" s="121" t="s">
-        <v>799</v>
+        <v>790</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="27" customFormat="1" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -8339,11 +8328,11 @@
         <v>26</v>
       </c>
       <c r="H3" s="30" t="s">
-        <v>806</v>
+        <v>797</v>
       </c>
       <c r="I3" s="30"/>
       <c r="J3" s="122" t="s">
-        <v>799</v>
+        <v>790</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="27" customFormat="1" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -8367,11 +8356,11 @@
         <v>26</v>
       </c>
       <c r="H4" s="30" t="s">
-        <v>807</v>
+        <v>798</v>
       </c>
       <c r="I4" s="30"/>
       <c r="J4" s="122" t="s">
-        <v>799</v>
+        <v>790</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="27" customFormat="1" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -8395,11 +8384,11 @@
         <v>26</v>
       </c>
       <c r="H5" s="30" t="s">
-        <v>808</v>
+        <v>799</v>
       </c>
       <c r="I5" s="30"/>
       <c r="J5" s="122" t="s">
-        <v>799</v>
+        <v>790</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="27" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -8423,11 +8412,11 @@
         <v>26</v>
       </c>
       <c r="H6" s="30" t="s">
-        <v>809</v>
+        <v>800</v>
       </c>
       <c r="I6" s="30"/>
       <c r="J6" s="122" t="s">
-        <v>799</v>
+        <v>790</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="27" customFormat="1" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -8451,11 +8440,11 @@
         <v>26</v>
       </c>
       <c r="H7" s="30" t="s">
-        <v>810</v>
+        <v>801</v>
       </c>
       <c r="I7" s="30"/>
       <c r="J7" s="122" t="s">
-        <v>799</v>
+        <v>790</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="27" customFormat="1" ht="141" thickBot="1" x14ac:dyDescent="0.35">
@@ -8503,11 +8492,11 @@
         <v>26</v>
       </c>
       <c r="H9" s="30" t="s">
-        <v>811</v>
+        <v>802</v>
       </c>
       <c r="I9" s="30"/>
       <c r="J9" s="122" t="s">
-        <v>801</v>
+        <v>792</v>
       </c>
     </row>
     <row r="10" spans="1:10" s="27" customFormat="1" ht="63" thickBot="1" x14ac:dyDescent="0.35">
@@ -8531,11 +8520,11 @@
         <v>26</v>
       </c>
       <c r="H10" s="30" t="s">
-        <v>812</v>
+        <v>803</v>
       </c>
       <c r="I10" s="30"/>
       <c r="J10" s="122" t="s">
-        <v>799</v>
+        <v>790</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="27" customFormat="1" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -8561,7 +8550,7 @@
       <c r="H11" s="30"/>
       <c r="I11" s="30"/>
       <c r="J11" s="122" t="s">
-        <v>799</v>
+        <v>790</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="27" customFormat="1" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -8585,11 +8574,11 @@
         <v>26</v>
       </c>
       <c r="H12" s="30" t="s">
-        <v>813</v>
+        <v>804</v>
       </c>
       <c r="I12" s="30"/>
       <c r="J12" s="34" t="s">
-        <v>801</v>
+        <v>792</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="27" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
@@ -8613,11 +8602,11 @@
         <v>26</v>
       </c>
       <c r="H13" s="30" t="s">
-        <v>814</v>
+        <v>805</v>
       </c>
       <c r="I13" s="30"/>
       <c r="J13" s="34" t="s">
-        <v>801</v>
+        <v>792</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="27" customFormat="1" ht="111" customHeight="1" x14ac:dyDescent="0.3">
@@ -8715,7 +8704,7 @@
       <c r="H17" s="30"/>
       <c r="I17" s="30"/>
       <c r="J17" s="34" t="s">
-        <v>802</v>
+        <v>793</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="27" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
@@ -8815,7 +8804,7 @@
       <c r="H21" s="30"/>
       <c r="I21" s="30"/>
       <c r="J21" s="34" t="s">
-        <v>803</v>
+        <v>794</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="27" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
@@ -8891,7 +8880,7 @@
       <c r="H24" s="30"/>
       <c r="I24" s="30"/>
       <c r="J24" s="34" t="s">
-        <v>800</v>
+        <v>791</v>
       </c>
     </row>
     <row r="25" spans="1:10" s="27" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
@@ -8917,7 +8906,7 @@
       <c r="H25" s="30"/>
       <c r="I25" s="30"/>
       <c r="J25" s="34" t="s">
-        <v>800</v>
+        <v>791</v>
       </c>
     </row>
     <row r="26" spans="1:10" s="27" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
@@ -8967,7 +8956,7 @@
       <c r="H27" s="30"/>
       <c r="I27" s="30"/>
       <c r="J27" s="34" t="s">
-        <v>800</v>
+        <v>791</v>
       </c>
     </row>
     <row r="28" spans="1:10" s="27" customFormat="1" ht="109.2" x14ac:dyDescent="0.3">
@@ -9043,7 +9032,7 @@
       <c r="H30" s="30"/>
       <c r="I30" s="30"/>
       <c r="J30" s="34" t="s">
-        <v>804</v>
+        <v>795</v>
       </c>
     </row>
     <row r="31" spans="1:10" s="27" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
@@ -9069,7 +9058,7 @@
       <c r="H31" s="30"/>
       <c r="I31" s="30"/>
       <c r="J31" s="34" t="s">
-        <v>804</v>
+        <v>795</v>
       </c>
     </row>
     <row r="32" spans="1:10" s="27" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
@@ -9095,7 +9084,7 @@
       <c r="H32" s="30"/>
       <c r="I32" s="30"/>
       <c r="J32" s="34" t="s">
-        <v>800</v>
+        <v>791</v>
       </c>
     </row>
     <row r="33" spans="1:10" s="27" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
@@ -9415,7 +9404,7 @@
       <c r="H45" s="30"/>
       <c r="I45" s="30"/>
       <c r="J45" s="34" t="s">
-        <v>799</v>
+        <v>790</v>
       </c>
     </row>
     <row r="46" spans="1:10" s="27" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
@@ -9441,7 +9430,7 @@
       <c r="H46" s="30"/>
       <c r="I46" s="30"/>
       <c r="J46" s="34" t="s">
-        <v>800</v>
+        <v>791</v>
       </c>
     </row>
     <row r="47" spans="1:10" s="27" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
@@ -9467,7 +9456,7 @@
       <c r="H47" s="30"/>
       <c r="I47" s="30"/>
       <c r="J47" s="34" t="s">
-        <v>800</v>
+        <v>791</v>
       </c>
     </row>
     <row r="48" spans="1:10" s="27" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
@@ -9493,7 +9482,7 @@
       <c r="H48" s="30"/>
       <c r="I48" s="30"/>
       <c r="J48" s="34" t="s">
-        <v>800</v>
+        <v>791</v>
       </c>
     </row>
     <row r="49" spans="1:10" s="27" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
@@ -9641,7 +9630,7 @@
       <c r="H54" s="30"/>
       <c r="I54" s="30"/>
       <c r="J54" s="34" t="s">
-        <v>800</v>
+        <v>791</v>
       </c>
     </row>
     <row r="55" spans="1:10" s="27" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -9669,7 +9658,7 @@
       <c r="H55" s="30"/>
       <c r="I55" s="30"/>
       <c r="J55" s="34" t="s">
-        <v>800</v>
+        <v>791</v>
       </c>
     </row>
     <row r="56" spans="1:10" s="27" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
@@ -9695,7 +9684,7 @@
       <c r="H56" s="30"/>
       <c r="I56" s="30"/>
       <c r="J56" s="34" t="s">
-        <v>800</v>
+        <v>791</v>
       </c>
     </row>
     <row r="57" spans="1:10" s="27" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
@@ -9721,7 +9710,7 @@
       <c r="H57" s="30"/>
       <c r="I57" s="30"/>
       <c r="J57" s="34" t="s">
-        <v>800</v>
+        <v>791</v>
       </c>
     </row>
     <row r="58" spans="1:10" s="27" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
@@ -9745,21 +9734,21 @@
       <c r="H58" s="40"/>
       <c r="I58" s="40"/>
       <c r="J58" s="43" t="s">
-        <v>800</v>
+        <v>791</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="A14:A20"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="A29:A35"/>
     <mergeCell ref="A36:A38"/>
     <mergeCell ref="A39:A44"/>
     <mergeCell ref="A45:A51"/>
     <mergeCell ref="A52:A54"/>
     <mergeCell ref="A55:A58"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="A14:A20"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A24:A28"/>
-    <mergeCell ref="A29:A35"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="G2:G58" xr:uid="{00000000-0002-0000-0200-000000000000}">
@@ -11304,7 +11293,7 @@
       <c r="I28" s="30"/>
       <c r="J28" s="34"/>
     </row>
-    <row r="29" spans="1:10" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" ht="78" x14ac:dyDescent="0.3">
       <c r="A29" s="124"/>
       <c r="B29" s="68" t="s">
         <v>455</v>

</xml_diff>

<commit_message>
#4 doc: asvs updated
</commit_message>
<xml_diff>
--- a/Deliverables/v4-ASVS-checklist-en.xlsx
+++ b/Deliverables/v4-ASVS-checklist-en.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dbeba1083b062d73/Ambiente de Trabalho/Desofs/desofs2024_m1b_2/Deliverables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodri\OneDrive\Documents\Mestrado\2Semestre\SISMD\PL3\desofs2024_m1b_2\Deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{7A4C5237-F738-468E-9773-D0E0FC29FDD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A66809D0-1EE3-4C95-9F1F-95C3160248D0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0616BB64-0C38-4662-A55D-678B3C94F299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" firstSheet="10" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ASVS Results" sheetId="1" r:id="rId1"/>
@@ -29,8 +29,19 @@
     <sheet name="API and Web Service" sheetId="14" r:id="rId14"/>
     <sheet name="Configuration" sheetId="15" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="181029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -39,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1313" uniqueCount="818">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1357" uniqueCount="849">
   <si>
     <t>Security Category</t>
   </si>
@@ -2465,36 +2476,6 @@
     <t>Sveltekit e Springboot</t>
   </si>
   <si>
-    <t>No frontend e backend foi implementado restrições de obrigar o utilizador a inserir uma palavra-passe superior ou igual a 12 caracteres</t>
-  </si>
-  <si>
-    <t>No frontend e backend garantimos que a password inserida poderia ter até 128 caracteres</t>
-  </si>
-  <si>
-    <t>No frontend e backend foi implementado uma função que substituia vários espaços por um único</t>
-  </si>
-  <si>
-    <t>O frontend e backend suportam nativamente esta funcionalidade</t>
-  </si>
-  <si>
-    <t>No frontend foi implementado uma página que em comunicação com o backend permite ao utilizador alterar a sua palavra-passe</t>
-  </si>
-  <si>
-    <t>Na página do frontend com comunicação com o backend tem 2 campos de inputs, um para a palavra-passe antiga e outro para a nova</t>
-  </si>
-  <si>
-    <t>No frontend enquanto o utilizador insere a nova palavra passe ou quando cria uma conta, tem uma medidor que atualiza em tempo real com o input que o utilizador insere</t>
-  </si>
-  <si>
-    <t>No frontend e backend não foi implementado nenhuma restrição relaciona a Uppercase, Lowercase e caracteres especiais</t>
-  </si>
-  <si>
-    <t>Esta funcionalidade encontra-se implementada nativamente</t>
-  </si>
-  <si>
-    <t>A funcionalidade foi implementada no frontend, em que o utilizador possui um botão para alterar a forma como visualiza a palavra-passe</t>
-  </si>
-  <si>
     <t>Através da biblioteca Apache Tika, verificou-se que os ficheiros enviados e recebidos apresentavam o encoding previsto</t>
   </si>
   <si>
@@ -2529,6 +2510,129 @@
   </si>
   <si>
     <t>O utlizador não consegue fazer pedidos diretos aos ficheiros</t>
+  </si>
+  <si>
+    <t>No frontend e backend foi implementado restrições de obrigar o utilizador a inserir uma palavra-passe superior ou igual a 12 caracteres. É possivel observar no useDTOSignup, e no +page.server.svelte da pagina de sigup</t>
+  </si>
+  <si>
+    <t>No frontend e backend garantimos que a password inserida poderia ter até 128 caracteres. É possivel observar no useDTOSignup, e no +page.server.svelte da pagina de sigup</t>
+  </si>
+  <si>
+    <t>No frontend e backend foi implementado uma função que substituia vários espaços por um único. É possivel observar na pagina de login e signup (+page.server.svelte).</t>
+  </si>
+  <si>
+    <t>O frontend e backend suportam nativamente esta funcionalidade.</t>
+  </si>
+  <si>
+    <t>No frontend foi implementado uma página que em comunicação com o backend permite ao utilizador alterar a sua palavra-passe. É possivel observar na pagina de trocar a password e no backend desde o userController até o userRepo</t>
+  </si>
+  <si>
+    <t>Na página do frontend com comunicação com o backend tem 2 campos de inputs, um para a palavra-passe antiga e outro para a nova. É possivel observar na pagina de trocar a password e no backend desde o userController até o userRepo</t>
+  </si>
+  <si>
+    <t>No frontend enquanto o utilizador insere a nova palavra passe ou quando cria uma conta, tem uma medidor que atualiza em tempo real com o input que o utilizador insere. Essa implementação é possivel ser observada na página do signup</t>
+  </si>
+  <si>
+    <t>No frontend e backend não foi implementado nenhuma restrição relaciona a Uppercase, Lowercase e caracteres especiais. É possivel observar no modelo user.java que não existe restrições desse tipo e no frontend (login e signup) tambem não</t>
+  </si>
+  <si>
+    <t>É possivel observar em todo a implementação que não existe rotação periódica de credenciais e históricod e palavra-passe como requisito</t>
+  </si>
+  <si>
+    <t>Esta funcionalidade encontra-se implementada nativamente.</t>
+  </si>
+  <si>
+    <t>A funcionalidade foi implementada no frontend, em que o utilizador possui um botão para alterar a forma como visualiza a palavra-passe. Essa funcionalidade é possivel de ser observada na pagina de login e signup (+page.svelte)</t>
+  </si>
+  <si>
+    <t>A funcionalidade foi implementada através do uso de criação de token e de ser necessitado o uso dela nas requests. É possivel observar no ficheiro AuthenticationAPI.java no backend</t>
+  </si>
+  <si>
+    <t>Não aplicamos porque não achamos seguro a palavra passe ser gerada automaticamente e enviada para o email. Basta o email do utilizador não ser seguro que a conta já se encontra comprometida</t>
+  </si>
+  <si>
+    <t>A funcionalidade foi implementada atraveés do uso de hashmd5, essa implementação é possivel ser observada na camada service das interações do user (login e signup)</t>
+  </si>
+  <si>
+    <t>Na linha 169 no ficheiro securityConfig.java bycrypt password enconder é possivel observar o numero do salt.</t>
+  </si>
+  <si>
+    <t>É possivel observar na linha 169 no ficheiro securityConfig o uso do bycript</t>
+  </si>
+  <si>
+    <t>Esta funcionalidade foi implementada e é possivel observar na AuthenticationAPI.java no backend</t>
+  </si>
+  <si>
+    <t>Esta funcionalidade está implementada nativamente pelos computadores e sistemas operativos atuais</t>
+  </si>
+  <si>
+    <t>Esta funcionaliadade é válida porque estamos a usar pbkdf2 e é possivel observar no backend</t>
+  </si>
+  <si>
+    <t>Esta funcionalidade é válida porque cada token gerado é único</t>
+  </si>
+  <si>
+    <t>Não é possivel implementar leitura biometrica em um website</t>
+  </si>
+  <si>
+    <t>Não é aplicavél por não termos conhecimento de uma fonte de dados que nos permita verificar se a palavra passe inserida pelo utilizador faz parte das mais usadas em todo o mundo</t>
+  </si>
+  <si>
+    <t>Não é aplicavél por não possuirmos conhecimento de uma possivel implementação do controlo de tentativa de automatização</t>
+  </si>
+  <si>
+    <t>Não é possivel porque não possuimos um serviço de emails/sms</t>
+  </si>
+  <si>
+    <t>Para ter um certificado de TLS verdadeiro e não pessoal, é preciso pagar, por isso não foi implementado</t>
+  </si>
+  <si>
+    <t>Não foi implementado porque não usamos one time passwords</t>
+  </si>
+  <si>
+    <t>Não foi implementado porq não possuirmos conhecimento sobre a área</t>
+  </si>
+  <si>
+    <t>Não foi implementado por falta de tempo</t>
+  </si>
+  <si>
+    <t>Não foi implementado as "secret questions" em toda a nossa solução</t>
+  </si>
+  <si>
+    <t>É possivel observar quer seja na pagina de alteração de password e no backend que a palavra passe atual não é mostrada em nenhum lugar</t>
+  </si>
+  <si>
+    <t>Não foi implementado OTP</t>
+  </si>
+  <si>
+    <t>A implementação foi feita em que nenhum local da nossa implementação temos alguma chave de a API ou palavra passes no código</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A palavra passe ao ser guardada na base de dados leva o processo de hash e não é possivel obter/visualizar a palavra-passe </t>
+  </si>
+  <si>
+    <t>Para aceder ao serviço é necessário inicialmente dar login com a password, e é possivel observar através da AuthenticationAPI.java</t>
+  </si>
+  <si>
+    <t>Não foi implementado porque optamos por outra alternativa</t>
+  </si>
+  <si>
+    <t>Não é possivel implementar porque não possuimos hardware para tal</t>
+  </si>
+  <si>
+    <t>Não foi implementado secrets</t>
+  </si>
+  <si>
+    <t>Não foi implementado por não possuir serviço de sms</t>
+  </si>
+  <si>
+    <t>Não foi implementado por não possuirmos conhecimento sobre o assunto</t>
+  </si>
+  <si>
+    <t>Não foi implementado porque não desenvolvemos um sistema de notificações de alterações no sistema</t>
+  </si>
+  <si>
+    <t>Foi implementado em que o backend não devolve um clear text mas sim uma response. É possivel observar no userController.java no backend</t>
   </si>
 </sst>
 </file>
@@ -3360,7 +3464,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3674,6 +3778,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -3683,11 +3793,14 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3871,7 +3984,7 @@
                     <a:latin typeface="Calibri"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="pt-PT"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -3945,13 +4058,13 @@
             <c:numRef>
               <c:f>'ASVS Results'!$D$2:$D$16</c:f>
               <c:numCache>
-                <c:formatCode>#\ ##0.00\ _€;\-#\ ##0.00\ _€</c:formatCode>
+                <c:formatCode>#,##0.00,_€;\-#,##0.00,_€</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>84.848484848484844</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>93.75</c:v>
+                  <c:v>96.551724137931032</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>71.428571428571431</c:v>
@@ -3990,7 +4103,7 @@
                   <c:v>90.476190476190482</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>81.730769230769226</c:v>
+                  <c:v>81.951219512195124</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4050,7 +4163,7 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="53282369"/>
@@ -4101,7 +4214,7 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="44868616"/>
@@ -4138,7 +4251,7 @@
               <a:latin typeface="Calibri"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4439,15 +4552,15 @@
       </c>
       <c r="B3" s="9">
         <f>COUNTIF(Authentication!G2:G58,"Valid")</f>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C3" s="10">
         <f>COUNTIF(Authentication!G2:G58,"&lt;&gt;Not Applicable")</f>
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D3" s="11">
         <f t="shared" si="0"/>
-        <v>93.75</v>
+        <v>96.551724137931032</v>
       </c>
       <c r="E3" s="12"/>
     </row>
@@ -4674,15 +4787,15 @@
       </c>
       <c r="B16" s="9">
         <f>SUM(B2:B15)</f>
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C16" s="10">
         <f>SUM(C2:C15)</f>
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D16" s="11">
         <f t="shared" si="0"/>
-        <v>81.730769230769226</v>
+        <v>81.951219512195124</v>
       </c>
       <c r="E16" s="12"/>
     </row>
@@ -4751,7 +4864,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="124" t="s">
+      <c r="A2" s="126" t="s">
         <v>561</v>
       </c>
       <c r="B2" s="68" t="s">
@@ -4775,7 +4888,7 @@
       <c r="J2" s="55"/>
     </row>
     <row r="3" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="124"/>
+      <c r="A3" s="126"/>
       <c r="B3" s="68" t="s">
         <v>564</v>
       </c>
@@ -4797,7 +4910,7 @@
       <c r="J3" s="34"/>
     </row>
     <row r="4" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="124"/>
+      <c r="A4" s="126"/>
       <c r="B4" s="68" t="s">
         <v>566</v>
       </c>
@@ -4819,7 +4932,7 @@
       <c r="J4" s="34"/>
     </row>
     <row r="5" spans="1:10" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="124" t="s">
+      <c r="A5" s="126" t="s">
         <v>568</v>
       </c>
       <c r="B5" s="68" t="s">
@@ -4843,7 +4956,7 @@
       <c r="J5" s="34"/>
     </row>
     <row r="6" spans="1:10" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="124"/>
+      <c r="A6" s="126"/>
       <c r="B6" s="68" t="s">
         <v>571</v>
       </c>
@@ -4865,7 +4978,7 @@
       <c r="J6" s="34"/>
     </row>
     <row r="7" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="124"/>
+      <c r="A7" s="126"/>
       <c r="B7" s="68" t="s">
         <v>573</v>
       </c>
@@ -4887,7 +5000,7 @@
       <c r="J7" s="34"/>
     </row>
     <row r="8" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="124"/>
+      <c r="A8" s="126"/>
       <c r="B8" s="68" t="s">
         <v>575</v>
       </c>
@@ -4909,7 +5022,7 @@
       <c r="J8" s="34"/>
     </row>
     <row r="9" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="124"/>
+      <c r="A9" s="126"/>
       <c r="B9" s="68" t="s">
         <v>577</v>
       </c>
@@ -5032,7 +5145,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="124" t="s">
+      <c r="A3" s="126" t="s">
         <v>584</v>
       </c>
       <c r="B3" s="68" t="s">
@@ -5058,7 +5171,7 @@
       <c r="J3" s="34"/>
     </row>
     <row r="4" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="124"/>
+      <c r="A4" s="126"/>
       <c r="B4" s="68" t="s">
         <v>588</v>
       </c>
@@ -5082,7 +5195,7 @@
       <c r="J4" s="34"/>
     </row>
     <row r="5" spans="1:10" ht="78" x14ac:dyDescent="0.3">
-      <c r="A5" s="124"/>
+      <c r="A5" s="126"/>
       <c r="B5" s="68" t="s">
         <v>591</v>
       </c>
@@ -5106,7 +5219,7 @@
       <c r="J5" s="34"/>
     </row>
     <row r="6" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="124"/>
+      <c r="A6" s="126"/>
       <c r="B6" s="68" t="s">
         <v>594</v>
       </c>
@@ -5130,7 +5243,7 @@
       <c r="J6" s="34"/>
     </row>
     <row r="7" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="124"/>
+      <c r="A7" s="126"/>
       <c r="B7" s="68" t="s">
         <v>597</v>
       </c>
@@ -5154,7 +5267,7 @@
       <c r="J7" s="34"/>
     </row>
     <row r="8" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="124"/>
+      <c r="A8" s="126"/>
       <c r="B8" s="68" t="s">
         <v>600</v>
       </c>
@@ -5178,7 +5291,7 @@
       <c r="J8" s="34"/>
     </row>
     <row r="9" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="124" t="s">
+      <c r="A9" s="126" t="s">
         <v>603</v>
       </c>
       <c r="B9" s="68" t="s">
@@ -5202,7 +5315,7 @@
       <c r="J9" s="34"/>
     </row>
     <row r="10" spans="1:10" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="124"/>
+      <c r="A10" s="126"/>
       <c r="B10" s="68" t="s">
         <v>606</v>
       </c>
@@ -5224,7 +5337,7 @@
       <c r="J10" s="34"/>
     </row>
     <row r="11" spans="1:10" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="124"/>
+      <c r="A11" s="126"/>
       <c r="B11" s="68" t="s">
         <v>608</v>
       </c>
@@ -5319,7 +5432,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="124" t="s">
+      <c r="A2" s="126" t="s">
         <v>610</v>
       </c>
       <c r="B2" s="68" t="s">
@@ -5345,7 +5458,7 @@
       <c r="J2" s="55"/>
     </row>
     <row r="3" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="124"/>
+      <c r="A3" s="126"/>
       <c r="B3" s="68" t="s">
         <v>614</v>
       </c>
@@ -5367,7 +5480,7 @@
       <c r="J3" s="34"/>
     </row>
     <row r="4" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="124"/>
+      <c r="A4" s="126"/>
       <c r="B4" s="68" t="s">
         <v>616</v>
       </c>
@@ -5389,7 +5502,7 @@
       <c r="J4" s="34"/>
     </row>
     <row r="5" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="124"/>
+      <c r="A5" s="126"/>
       <c r="B5" s="68" t="s">
         <v>618</v>
       </c>
@@ -5411,7 +5524,7 @@
       <c r="J5" s="34"/>
     </row>
     <row r="6" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="124"/>
+      <c r="A6" s="126"/>
       <c r="B6" s="68" t="s">
         <v>620</v>
       </c>
@@ -5433,7 +5546,7 @@
       <c r="J6" s="34"/>
     </row>
     <row r="7" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="124"/>
+      <c r="A7" s="126"/>
       <c r="B7" s="68" t="s">
         <v>622</v>
       </c>
@@ -5453,7 +5566,7 @@
       <c r="J7" s="34"/>
     </row>
     <row r="8" spans="1:10" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="124"/>
+      <c r="A8" s="126"/>
       <c r="B8" s="68" t="s">
         <v>624</v>
       </c>
@@ -5475,7 +5588,7 @@
       <c r="J8" s="34"/>
     </row>
     <row r="9" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="124"/>
+      <c r="A9" s="126"/>
       <c r="B9" s="68" t="s">
         <v>626</v>
       </c>
@@ -5519,8 +5632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:AMJ16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -5569,7 +5682,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="63" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="124" t="s">
+      <c r="A2" s="126" t="s">
         <v>628</v>
       </c>
       <c r="B2" s="68" t="s">
@@ -5589,13 +5702,13 @@
         <v>26</v>
       </c>
       <c r="H2" s="117" t="s">
-        <v>807</v>
+        <v>797</v>
       </c>
       <c r="I2" s="54"/>
       <c r="J2" s="55"/>
     </row>
     <row r="3" spans="1:10" ht="78.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="124"/>
+      <c r="A3" s="126"/>
       <c r="B3" s="68" t="s">
         <v>631</v>
       </c>
@@ -5614,12 +5727,12 @@
       </c>
       <c r="H3" s="30"/>
       <c r="I3" s="32" t="s">
-        <v>814</v>
+        <v>804</v>
       </c>
       <c r="J3" s="34"/>
     </row>
     <row r="4" spans="1:10" ht="63" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="124"/>
+      <c r="A4" s="126"/>
       <c r="B4" s="68" t="s">
         <v>633</v>
       </c>
@@ -5637,7 +5750,7 @@
         <v>26</v>
       </c>
       <c r="H4" s="32" t="s">
-        <v>808</v>
+        <v>798</v>
       </c>
       <c r="I4" s="30"/>
       <c r="J4" s="34"/>
@@ -5663,13 +5776,13 @@
         <v>26</v>
       </c>
       <c r="H5" s="32" t="s">
-        <v>809</v>
+        <v>799</v>
       </c>
       <c r="I5" s="30"/>
       <c r="J5" s="34"/>
     </row>
     <row r="6" spans="1:10" ht="63" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="124" t="s">
+      <c r="A6" s="126" t="s">
         <v>638</v>
       </c>
       <c r="B6" s="68" t="s">
@@ -5689,13 +5802,13 @@
         <v>26</v>
       </c>
       <c r="H6" s="32" t="s">
-        <v>810</v>
+        <v>800</v>
       </c>
       <c r="I6" s="30"/>
       <c r="J6" s="34"/>
     </row>
     <row r="7" spans="1:10" ht="63" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="124"/>
+      <c r="A7" s="126"/>
       <c r="B7" s="68" t="s">
         <v>641</v>
       </c>
@@ -5713,13 +5826,13 @@
         <v>26</v>
       </c>
       <c r="H7" s="32" t="s">
-        <v>810</v>
+        <v>800</v>
       </c>
       <c r="I7" s="30"/>
       <c r="J7" s="34"/>
     </row>
     <row r="8" spans="1:10" ht="63" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="124"/>
+      <c r="A8" s="126"/>
       <c r="B8" s="68" t="s">
         <v>643</v>
       </c>
@@ -5737,13 +5850,13 @@
         <v>26</v>
       </c>
       <c r="H8" s="32" t="s">
-        <v>810</v>
+        <v>800</v>
       </c>
       <c r="I8" s="30"/>
       <c r="J8" s="34"/>
     </row>
     <row r="9" spans="1:10" ht="172.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="124"/>
+      <c r="A9" s="126"/>
       <c r="B9" s="68" t="s">
         <v>645</v>
       </c>
@@ -5757,17 +5870,17 @@
       <c r="F9" s="31" t="s">
         <v>646</v>
       </c>
-      <c r="G9" s="126" t="s">
+      <c r="G9" s="123" t="s">
         <v>61</v>
       </c>
       <c r="H9" s="120"/>
       <c r="I9" s="32" t="s">
-        <v>815</v>
+        <v>805</v>
       </c>
       <c r="J9" s="34"/>
     </row>
     <row r="10" spans="1:10" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="124"/>
+      <c r="A10" s="126"/>
       <c r="B10" s="68" t="s">
         <v>647</v>
       </c>
@@ -5789,7 +5902,7 @@
       <c r="J10" s="34"/>
     </row>
     <row r="11" spans="1:10" ht="63" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="124"/>
+      <c r="A11" s="126"/>
       <c r="B11" s="68" t="s">
         <v>649</v>
       </c>
@@ -5807,13 +5920,13 @@
         <v>26</v>
       </c>
       <c r="H11" s="32" t="s">
-        <v>813</v>
+        <v>803</v>
       </c>
       <c r="I11" s="30"/>
       <c r="J11" s="34"/>
     </row>
     <row r="12" spans="1:10" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="124" t="s">
+      <c r="A12" s="126" t="s">
         <v>651</v>
       </c>
       <c r="B12" s="68" t="s">
@@ -5833,13 +5946,13 @@
         <v>26</v>
       </c>
       <c r="H12" s="32" t="s">
-        <v>811</v>
+        <v>801</v>
       </c>
       <c r="I12" s="30"/>
       <c r="J12" s="34"/>
     </row>
     <row r="13" spans="1:10" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="124"/>
+      <c r="A13" s="126"/>
       <c r="B13" s="68" t="s">
         <v>654</v>
       </c>
@@ -5861,7 +5974,7 @@
       <c r="J13" s="34"/>
     </row>
     <row r="14" spans="1:10" ht="94.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="124" t="s">
+      <c r="A14" s="126" t="s">
         <v>656</v>
       </c>
       <c r="B14" s="68" t="s">
@@ -5881,13 +5994,13 @@
         <v>26</v>
       </c>
       <c r="H14" s="119" t="s">
-        <v>812</v>
+        <v>802</v>
       </c>
       <c r="I14" s="30"/>
       <c r="J14" s="34"/>
     </row>
     <row r="15" spans="1:10" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="124"/>
+      <c r="A15" s="126"/>
       <c r="B15" s="68" t="s">
         <v>659</v>
       </c>
@@ -5906,7 +6019,7 @@
       </c>
       <c r="H15" s="30"/>
       <c r="I15" s="31" t="s">
-        <v>817</v>
+        <v>807</v>
       </c>
       <c r="J15" s="34"/>
     </row>
@@ -5924,14 +6037,14 @@
         <v>918</v>
       </c>
       <c r="E16" s="39"/>
-      <c r="F16" s="127" t="s">
+      <c r="F16" s="124" t="s">
         <v>663</v>
       </c>
       <c r="G16" s="40" t="s">
         <v>26</v>
       </c>
       <c r="H16" s="80" t="s">
-        <v>816</v>
+        <v>806</v>
       </c>
       <c r="I16" s="40"/>
       <c r="J16" s="43"/>
@@ -6011,7 +6124,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="124" t="s">
+      <c r="A2" s="126" t="s">
         <v>664</v>
       </c>
       <c r="B2" s="68" t="s">
@@ -6031,13 +6144,13 @@
         <v>26</v>
       </c>
       <c r="H2" s="118" t="s">
-        <v>806</v>
+        <v>796</v>
       </c>
       <c r="I2" s="54"/>
       <c r="J2" s="55"/>
     </row>
     <row r="3" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="124"/>
+      <c r="A3" s="126"/>
       <c r="B3" s="68" t="s">
         <v>667</v>
       </c>
@@ -6059,7 +6172,7 @@
       <c r="J3" s="34"/>
     </row>
     <row r="4" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="124"/>
+      <c r="A4" s="126"/>
       <c r="B4" s="68" t="s">
         <v>669</v>
       </c>
@@ -6083,7 +6196,7 @@
       <c r="J4" s="34"/>
     </row>
     <row r="5" spans="1:10" ht="171.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="124"/>
+      <c r="A5" s="126"/>
       <c r="B5" s="68" t="s">
         <v>672</v>
       </c>
@@ -6109,7 +6222,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="124"/>
+      <c r="A6" s="126"/>
       <c r="B6" s="68" t="s">
         <v>676</v>
       </c>
@@ -6133,7 +6246,7 @@
       <c r="J6" s="34"/>
     </row>
     <row r="7" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="124" t="s">
+      <c r="A7" s="126" t="s">
         <v>679</v>
       </c>
       <c r="B7" s="68" t="s">
@@ -6159,7 +6272,7 @@
       <c r="J7" s="34"/>
     </row>
     <row r="8" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="124"/>
+      <c r="A8" s="126"/>
       <c r="B8" s="68" t="s">
         <v>683</v>
       </c>
@@ -6183,7 +6296,7 @@
       <c r="J8" s="34"/>
     </row>
     <row r="9" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="124"/>
+      <c r="A9" s="126"/>
       <c r="B9" s="68" t="s">
         <v>686</v>
       </c>
@@ -6205,7 +6318,7 @@
       <c r="J9" s="34"/>
     </row>
     <row r="10" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="124"/>
+      <c r="A10" s="126"/>
       <c r="B10" s="68" t="s">
         <v>688</v>
       </c>
@@ -6227,7 +6340,7 @@
       <c r="J10" s="34"/>
     </row>
     <row r="11" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="124"/>
+      <c r="A11" s="126"/>
       <c r="B11" s="68" t="s">
         <v>690</v>
       </c>
@@ -6251,7 +6364,7 @@
       <c r="J11" s="34"/>
     </row>
     <row r="12" spans="1:10" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="124"/>
+      <c r="A12" s="126"/>
       <c r="B12" s="68" t="s">
         <v>693</v>
       </c>
@@ -6273,7 +6386,7 @@
       <c r="J12" s="34"/>
     </row>
     <row r="13" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="124" t="s">
+      <c r="A13" s="126" t="s">
         <v>695</v>
       </c>
       <c r="B13" s="68" t="s">
@@ -6299,7 +6412,7 @@
       <c r="J13" s="34"/>
     </row>
     <row r="14" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="124"/>
+      <c r="A14" s="126"/>
       <c r="B14" s="68" t="s">
         <v>699</v>
       </c>
@@ -6321,7 +6434,7 @@
       <c r="J14" s="34"/>
     </row>
     <row r="15" spans="1:10" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="124" t="s">
+      <c r="A15" s="126" t="s">
         <v>701</v>
       </c>
       <c r="B15" s="68" t="s">
@@ -6345,7 +6458,7 @@
       <c r="J15" s="34"/>
     </row>
     <row r="16" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="124"/>
+      <c r="A16" s="126"/>
       <c r="B16" s="68" t="s">
         <v>704</v>
       </c>
@@ -6442,7 +6555,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="125" t="s">
+      <c r="A2" s="127" t="s">
         <v>706</v>
       </c>
       <c r="B2" s="97" t="s">
@@ -6468,7 +6581,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="125"/>
+      <c r="A3" s="127"/>
       <c r="B3" s="68" t="s">
         <v>711</v>
       </c>
@@ -6492,7 +6605,7 @@
       <c r="J3" s="107"/>
     </row>
     <row r="4" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="125"/>
+      <c r="A4" s="127"/>
       <c r="B4" s="68" t="s">
         <v>714</v>
       </c>
@@ -6518,7 +6631,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="125"/>
+      <c r="A5" s="127"/>
       <c r="B5" s="68" t="s">
         <v>718</v>
       </c>
@@ -6542,7 +6655,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="125"/>
+      <c r="A6" s="127"/>
       <c r="B6" s="68" t="s">
         <v>721</v>
       </c>
@@ -6566,7 +6679,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="124" t="s">
+      <c r="A7" s="126" t="s">
         <v>725</v>
       </c>
       <c r="B7" s="68" t="s">
@@ -6594,7 +6707,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="124"/>
+      <c r="A8" s="126"/>
       <c r="B8" s="68" t="s">
         <v>730</v>
       </c>
@@ -6618,7 +6731,7 @@
       <c r="J8" s="107"/>
     </row>
     <row r="9" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="124"/>
+      <c r="A9" s="126"/>
       <c r="B9" s="68" t="s">
         <v>733</v>
       </c>
@@ -6642,7 +6755,7 @@
       <c r="J9" s="107"/>
     </row>
     <row r="10" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="124"/>
+      <c r="A10" s="126"/>
       <c r="B10" s="68" t="s">
         <v>736</v>
       </c>
@@ -6666,7 +6779,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="124"/>
+      <c r="A11" s="126"/>
       <c r="B11" s="68" t="s">
         <v>740</v>
       </c>
@@ -6686,7 +6799,7 @@
       <c r="J11" s="107"/>
     </row>
     <row r="12" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="124"/>
+      <c r="A12" s="126"/>
       <c r="B12" s="68" t="s">
         <v>742</v>
       </c>
@@ -6710,7 +6823,7 @@
       <c r="J12" s="107"/>
     </row>
     <row r="13" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="124" t="s">
+      <c r="A13" s="126" t="s">
         <v>745</v>
       </c>
       <c r="B13" s="68" t="s">
@@ -6734,7 +6847,7 @@
       <c r="J13" s="107"/>
     </row>
     <row r="14" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="124"/>
+      <c r="A14" s="126"/>
       <c r="B14" s="68" t="s">
         <v>748</v>
       </c>
@@ -6758,7 +6871,7 @@
       <c r="J14" s="107"/>
     </row>
     <row r="15" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="124"/>
+      <c r="A15" s="126"/>
       <c r="B15" s="68" t="s">
         <v>751</v>
       </c>
@@ -6782,7 +6895,7 @@
       <c r="J15" s="107"/>
     </row>
     <row r="16" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="124" t="s">
+      <c r="A16" s="126" t="s">
         <v>754</v>
       </c>
       <c r="B16" s="68" t="s">
@@ -6810,7 +6923,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="124"/>
+      <c r="A17" s="126"/>
       <c r="B17" s="68" t="s">
         <v>759</v>
       </c>
@@ -6834,7 +6947,7 @@
       <c r="J17" s="107"/>
     </row>
     <row r="18" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="124"/>
+      <c r="A18" s="126"/>
       <c r="B18" s="68" t="s">
         <v>762</v>
       </c>
@@ -6856,7 +6969,7 @@
       <c r="J18" s="107"/>
     </row>
     <row r="19" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="124"/>
+      <c r="A19" s="126"/>
       <c r="B19" s="68" t="s">
         <v>764</v>
       </c>
@@ -6882,7 +6995,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="124"/>
+      <c r="A20" s="126"/>
       <c r="B20" s="68" t="s">
         <v>768</v>
       </c>
@@ -6906,7 +7019,7 @@
       <c r="J20" s="107"/>
     </row>
     <row r="21" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="124"/>
+      <c r="A21" s="126"/>
       <c r="B21" s="68" t="s">
         <v>771</v>
       </c>
@@ -6930,7 +7043,7 @@
       <c r="J21" s="107"/>
     </row>
     <row r="22" spans="1:10" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A22" s="124"/>
+      <c r="A22" s="126"/>
       <c r="B22" s="68" t="s">
         <v>774</v>
       </c>
@@ -6952,7 +7065,7 @@
       <c r="J22" s="107"/>
     </row>
     <row r="23" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="124" t="s">
+      <c r="A23" s="126" t="s">
         <v>776</v>
       </c>
       <c r="B23" s="68" t="s">
@@ -6978,7 +7091,7 @@
       <c r="J23" s="107"/>
     </row>
     <row r="24" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="124"/>
+      <c r="A24" s="126"/>
       <c r="B24" s="68" t="s">
         <v>780</v>
       </c>
@@ -7002,7 +7115,7 @@
       <c r="J24" s="107"/>
     </row>
     <row r="25" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="124"/>
+      <c r="A25" s="126"/>
       <c r="B25" s="68" t="s">
         <v>783</v>
       </c>
@@ -7026,7 +7139,7 @@
       <c r="J25" s="107"/>
     </row>
     <row r="26" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A26" s="124"/>
+      <c r="A26" s="126"/>
       <c r="B26" s="68" t="s">
         <v>787</v>
       </c>
@@ -7130,7 +7243,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" s="27" customFormat="1" ht="97.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="123" t="s">
+      <c r="A2" s="125" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="20" t="s">
@@ -7156,7 +7269,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" s="27" customFormat="1" ht="234" x14ac:dyDescent="0.3">
-      <c r="A3" s="123"/>
+      <c r="A3" s="125"/>
       <c r="B3" s="20" t="s">
         <v>35</v>
       </c>
@@ -7184,7 +7297,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" s="27" customFormat="1" ht="140.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="123"/>
+      <c r="A4" s="125"/>
       <c r="B4" s="20" t="s">
         <v>40</v>
       </c>
@@ -7208,7 +7321,7 @@
       <c r="J4" s="34"/>
     </row>
     <row r="5" spans="1:10" s="27" customFormat="1" ht="109.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="123"/>
+      <c r="A5" s="125"/>
       <c r="B5" s="20" t="s">
         <v>43</v>
       </c>
@@ -7234,7 +7347,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" s="27" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="123"/>
+      <c r="A6" s="125"/>
       <c r="B6" s="20" t="s">
         <v>46</v>
       </c>
@@ -7260,7 +7373,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" s="27" customFormat="1" ht="124.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="123"/>
+      <c r="A7" s="125"/>
       <c r="B7" s="20" t="s">
         <v>49</v>
       </c>
@@ -7286,7 +7399,7 @@
       <c r="J7" s="34"/>
     </row>
     <row r="8" spans="1:10" s="27" customFormat="1" ht="109.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="123"/>
+      <c r="A8" s="125"/>
       <c r="B8" s="20" t="s">
         <v>53</v>
       </c>
@@ -7314,7 +7427,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" s="27" customFormat="1" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="123" t="s">
+      <c r="A9" s="125" t="s">
         <v>58</v>
       </c>
       <c r="B9" s="20" t="s">
@@ -7340,7 +7453,7 @@
       <c r="J9" s="34"/>
     </row>
     <row r="10" spans="1:10" s="27" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="123"/>
+      <c r="A10" s="125"/>
       <c r="B10" s="20" t="s">
         <v>63</v>
       </c>
@@ -7364,7 +7477,7 @@
       <c r="J10" s="34"/>
     </row>
     <row r="11" spans="1:10" s="27" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="123"/>
+      <c r="A11" s="125"/>
       <c r="B11" s="20" t="s">
         <v>66</v>
       </c>
@@ -7390,7 +7503,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" s="27" customFormat="1" ht="124.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="123"/>
+      <c r="A12" s="125"/>
       <c r="B12" s="20" t="s">
         <v>70</v>
       </c>
@@ -7434,7 +7547,7 @@
       <c r="J13" s="34"/>
     </row>
     <row r="14" spans="1:10" s="27" customFormat="1" ht="108.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="123" t="s">
+      <c r="A14" s="125" t="s">
         <v>76</v>
       </c>
       <c r="B14" s="20" t="s">
@@ -7462,7 +7575,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" s="27" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="123"/>
+      <c r="A15" s="125"/>
       <c r="B15" s="20" t="s">
         <v>81</v>
       </c>
@@ -7484,7 +7597,7 @@
       <c r="J15" s="34"/>
     </row>
     <row r="16" spans="1:10" s="27" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="123"/>
+      <c r="A16" s="125"/>
       <c r="B16" s="20" t="s">
         <v>83</v>
       </c>
@@ -7506,7 +7619,7 @@
       <c r="J16" s="34"/>
     </row>
     <row r="17" spans="1:10" s="27" customFormat="1" ht="109.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="123"/>
+      <c r="A17" s="125"/>
       <c r="B17" s="20" t="s">
         <v>85</v>
       </c>
@@ -7530,7 +7643,7 @@
       <c r="J17" s="34"/>
     </row>
     <row r="18" spans="1:10" s="27" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="123"/>
+      <c r="A18" s="125"/>
       <c r="B18" s="20" t="s">
         <v>88</v>
       </c>
@@ -7554,7 +7667,7 @@
       <c r="J18" s="34"/>
     </row>
     <row r="19" spans="1:10" s="27" customFormat="1" ht="37.35" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="123" t="s">
+      <c r="A19" s="125" t="s">
         <v>92</v>
       </c>
       <c r="B19" s="20" t="s">
@@ -7580,7 +7693,7 @@
       <c r="J19" s="34"/>
     </row>
     <row r="20" spans="1:10" s="27" customFormat="1" ht="78" x14ac:dyDescent="0.3">
-      <c r="A20" s="123"/>
+      <c r="A20" s="125"/>
       <c r="B20" s="20" t="s">
         <v>96</v>
       </c>
@@ -7604,7 +7717,7 @@
       <c r="J20" s="34"/>
     </row>
     <row r="21" spans="1:10" s="27" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A21" s="123"/>
+      <c r="A21" s="125"/>
       <c r="B21" s="20" t="s">
         <v>99</v>
       </c>
@@ -7630,7 +7743,7 @@
       </c>
     </row>
     <row r="22" spans="1:10" s="27" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A22" s="123"/>
+      <c r="A22" s="125"/>
       <c r="B22" s="20" t="s">
         <v>103</v>
       </c>
@@ -7654,7 +7767,7 @@
       <c r="J22" s="34"/>
     </row>
     <row r="23" spans="1:10" s="27" customFormat="1" ht="37.35" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="123" t="s">
+      <c r="A23" s="125" t="s">
         <v>106</v>
       </c>
       <c r="B23" s="20" t="s">
@@ -7680,7 +7793,7 @@
       <c r="J23" s="34"/>
     </row>
     <row r="24" spans="1:10" s="27" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A24" s="123"/>
+      <c r="A24" s="125"/>
       <c r="B24" s="20" t="s">
         <v>110</v>
       </c>
@@ -7704,7 +7817,7 @@
       <c r="J24" s="34"/>
     </row>
     <row r="25" spans="1:10" s="27" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A25" s="123"/>
+      <c r="A25" s="125"/>
       <c r="B25" s="20" t="s">
         <v>113</v>
       </c>
@@ -7728,7 +7841,7 @@
       <c r="J25" s="34"/>
     </row>
     <row r="26" spans="1:10" s="27" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A26" s="123"/>
+      <c r="A26" s="125"/>
       <c r="B26" s="20" t="s">
         <v>116</v>
       </c>
@@ -7754,7 +7867,7 @@
       <c r="J26" s="34"/>
     </row>
     <row r="27" spans="1:10" s="27" customFormat="1" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="123" t="s">
+      <c r="A27" s="125" t="s">
         <v>120</v>
       </c>
       <c r="B27" s="20" t="s">
@@ -7782,7 +7895,7 @@
       <c r="J27" s="34"/>
     </row>
     <row r="28" spans="1:10" s="27" customFormat="1" ht="124.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="123"/>
+      <c r="A28" s="125"/>
       <c r="B28" s="20" t="s">
         <v>125</v>
       </c>
@@ -7804,7 +7917,7 @@
       <c r="J28" s="34"/>
     </row>
     <row r="29" spans="1:10" s="27" customFormat="1" ht="37.35" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="123" t="s">
+      <c r="A29" s="125" t="s">
         <v>128</v>
       </c>
       <c r="B29" s="20" t="s">
@@ -7828,7 +7941,7 @@
       <c r="J29" s="34"/>
     </row>
     <row r="30" spans="1:10" s="27" customFormat="1" ht="78" x14ac:dyDescent="0.3">
-      <c r="A30" s="123"/>
+      <c r="A30" s="125"/>
       <c r="B30" s="20" t="s">
         <v>132</v>
       </c>
@@ -7850,7 +7963,7 @@
       <c r="J30" s="34"/>
     </row>
     <row r="31" spans="1:10" s="27" customFormat="1" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="123" t="s">
+      <c r="A31" s="125" t="s">
         <v>135</v>
       </c>
       <c r="B31" s="20" t="s">
@@ -7876,7 +7989,7 @@
       <c r="J31" s="34"/>
     </row>
     <row r="32" spans="1:10" s="27" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A32" s="123"/>
+      <c r="A32" s="125"/>
       <c r="B32" s="20" t="s">
         <v>139</v>
       </c>
@@ -7928,7 +8041,7 @@
       </c>
     </row>
     <row r="34" spans="1:10" s="27" customFormat="1" ht="52.2" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="123" t="s">
+      <c r="A34" s="125" t="s">
         <v>147</v>
       </c>
       <c r="B34" s="20" t="s">
@@ -7954,7 +8067,7 @@
       <c r="J34" s="34"/>
     </row>
     <row r="35" spans="1:10" s="27" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A35" s="123"/>
+      <c r="A35" s="125"/>
       <c r="B35" s="20" t="s">
         <v>151</v>
       </c>
@@ -7978,7 +8091,7 @@
       <c r="J35" s="34"/>
     </row>
     <row r="36" spans="1:10" s="27" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A36" s="123"/>
+      <c r="A36" s="125"/>
       <c r="B36" s="20" t="s">
         <v>154</v>
       </c>
@@ -8002,7 +8115,7 @@
       <c r="J36" s="34"/>
     </row>
     <row r="37" spans="1:10" s="27" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="123" t="s">
+      <c r="A37" s="125" t="s">
         <v>157</v>
       </c>
       <c r="B37" s="20" t="s">
@@ -8026,7 +8139,7 @@
       <c r="J37" s="34"/>
     </row>
     <row r="38" spans="1:10" s="27" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="123"/>
+      <c r="A38" s="125"/>
       <c r="B38" s="20" t="s">
         <v>160</v>
       </c>
@@ -8066,7 +8179,7 @@
       <c r="J39" s="34"/>
     </row>
     <row r="40" spans="1:10" s="27" customFormat="1" ht="52.2" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="123" t="s">
+      <c r="A40" s="125" t="s">
         <v>164</v>
       </c>
       <c r="B40" s="20" t="s">
@@ -8092,7 +8205,7 @@
       <c r="J40" s="34"/>
     </row>
     <row r="41" spans="1:10" s="27" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A41" s="123"/>
+      <c r="A41" s="125"/>
       <c r="B41" s="20" t="s">
         <v>168</v>
       </c>
@@ -8116,7 +8229,7 @@
       <c r="J41" s="34"/>
     </row>
     <row r="42" spans="1:10" s="27" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="123"/>
+      <c r="A42" s="125"/>
       <c r="B42" s="20" t="s">
         <v>170</v>
       </c>
@@ -8142,7 +8255,7 @@
       </c>
     </row>
     <row r="43" spans="1:10" s="27" customFormat="1" ht="78" x14ac:dyDescent="0.3">
-      <c r="A43" s="123"/>
+      <c r="A43" s="125"/>
       <c r="B43" s="20" t="s">
         <v>174</v>
       </c>
@@ -8164,7 +8277,7 @@
       <c r="J43" s="34"/>
     </row>
     <row r="44" spans="1:10" s="27" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="123"/>
+      <c r="A44" s="125"/>
       <c r="B44" s="20" t="s">
         <v>177</v>
       </c>
@@ -8190,7 +8303,7 @@
       </c>
     </row>
     <row r="45" spans="1:10" s="27" customFormat="1" ht="66.599999999999994" x14ac:dyDescent="0.3">
-      <c r="A45" s="123"/>
+      <c r="A45" s="125"/>
       <c r="B45" s="20" t="s">
         <v>181</v>
       </c>
@@ -8217,17 +8330,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A23:A26"/>
     <mergeCell ref="A40:A45"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="A29:A30"/>
     <mergeCell ref="A31:A32"/>
     <mergeCell ref="A34:A36"/>
     <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A23:A26"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="G2:G45" xr:uid="{00000000-0002-0000-0100-000000000000}">
@@ -8248,8 +8361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMJ58"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -8260,8 +8373,8 @@
     <col min="4" max="5" width="8.88671875" style="44"/>
     <col min="6" max="6" width="73" style="15" customWidth="1"/>
     <col min="7" max="7" width="25.44140625" style="15" customWidth="1"/>
-    <col min="8" max="8" width="30.21875" style="15" customWidth="1"/>
-    <col min="9" max="9" width="33.44140625" style="15" customWidth="1"/>
+    <col min="8" max="8" width="30.21875" style="130" customWidth="1"/>
+    <col min="9" max="9" width="33.44140625" style="130" customWidth="1"/>
     <col min="10" max="10" width="29" style="15" customWidth="1"/>
     <col min="11" max="1024" width="8.88671875" style="15"/>
   </cols>
@@ -8288,10 +8401,10 @@
       <c r="G1" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="47" t="s">
+      <c r="H1" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="47" t="s">
+      <c r="I1" s="46" t="s">
         <v>28</v>
       </c>
       <c r="J1" s="47" t="s">
@@ -8299,7 +8412,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" s="27" customFormat="1" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="124" t="s">
+      <c r="A2" s="126" t="s">
         <v>185</v>
       </c>
       <c r="B2" s="49" t="s">
@@ -8320,16 +8433,16 @@
       <c r="G2" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="54" t="s">
-        <v>796</v>
-      </c>
-      <c r="I2" s="54"/>
+      <c r="H2" s="117" t="s">
+        <v>808</v>
+      </c>
+      <c r="I2" s="117"/>
       <c r="J2" s="121" t="s">
         <v>790</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="27" customFormat="1" ht="63" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="124"/>
+    <row r="3" spans="1:10" s="27" customFormat="1" ht="109.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="126"/>
       <c r="B3" s="49" t="s">
         <v>189</v>
       </c>
@@ -8348,16 +8461,16 @@
       <c r="G3" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="30" t="s">
-        <v>797</v>
-      </c>
-      <c r="I3" s="30"/>
+      <c r="H3" s="32" t="s">
+        <v>809</v>
+      </c>
+      <c r="I3" s="32"/>
       <c r="J3" s="122" t="s">
         <v>790</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="27" customFormat="1" ht="63" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="124"/>
+    <row r="4" spans="1:10" s="27" customFormat="1" ht="94.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="126"/>
       <c r="B4" s="49" t="s">
         <v>191</v>
       </c>
@@ -8376,16 +8489,16 @@
       <c r="G4" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="30" t="s">
-        <v>798</v>
-      </c>
-      <c r="I4" s="30"/>
+      <c r="H4" s="32" t="s">
+        <v>810</v>
+      </c>
+      <c r="I4" s="32"/>
       <c r="J4" s="122" t="s">
         <v>790</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="27" customFormat="1" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="124"/>
+    <row r="5" spans="1:10" s="27" customFormat="1" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="126"/>
       <c r="B5" s="49" t="s">
         <v>193</v>
       </c>
@@ -8404,16 +8517,16 @@
       <c r="G5" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="30" t="s">
-        <v>799</v>
-      </c>
-      <c r="I5" s="30"/>
+      <c r="H5" s="32" t="s">
+        <v>811</v>
+      </c>
+      <c r="I5" s="32"/>
       <c r="J5" s="122" t="s">
         <v>790</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="27" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="124"/>
+    <row r="6" spans="1:10" s="27" customFormat="1" ht="141" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="126"/>
       <c r="B6" s="49" t="s">
         <v>195</v>
       </c>
@@ -8432,16 +8545,16 @@
       <c r="G6" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="30" t="s">
-        <v>800</v>
-      </c>
-      <c r="I6" s="30"/>
+      <c r="H6" s="32" t="s">
+        <v>812</v>
+      </c>
+      <c r="I6" s="32"/>
       <c r="J6" s="122" t="s">
         <v>790</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="27" customFormat="1" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="124"/>
+    <row r="7" spans="1:10" s="27" customFormat="1" ht="141" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="126"/>
       <c r="B7" s="49" t="s">
         <v>197</v>
       </c>
@@ -8460,16 +8573,16 @@
       <c r="G7" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="30" t="s">
-        <v>801</v>
-      </c>
-      <c r="I7" s="30"/>
+      <c r="H7" s="32" t="s">
+        <v>813</v>
+      </c>
+      <c r="I7" s="32"/>
       <c r="J7" s="122" t="s">
         <v>790</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="27" customFormat="1" ht="156.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="124"/>
+    <row r="8" spans="1:10" s="27" customFormat="1" ht="141" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="126"/>
       <c r="B8" s="49" t="s">
         <v>199</v>
       </c>
@@ -8488,12 +8601,14 @@
       <c r="G8" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
+      <c r="H8" s="128"/>
+      <c r="I8" s="32" t="s">
+        <v>829</v>
+      </c>
       <c r="J8" s="122"/>
     </row>
-    <row r="9" spans="1:10" s="27" customFormat="1" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="124"/>
+    <row r="9" spans="1:10" s="27" customFormat="1" ht="141" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="126"/>
       <c r="B9" s="49" t="s">
         <v>201</v>
       </c>
@@ -8512,16 +8627,16 @@
       <c r="G9" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="30" t="s">
-        <v>802</v>
-      </c>
-      <c r="I9" s="30"/>
+      <c r="H9" s="32" t="s">
+        <v>814</v>
+      </c>
+      <c r="I9" s="32"/>
       <c r="J9" s="122" t="s">
         <v>792</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="27" customFormat="1" ht="63" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="124"/>
+    <row r="10" spans="1:10" s="27" customFormat="1" ht="156.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="126"/>
       <c r="B10" s="49" t="s">
         <v>203</v>
       </c>
@@ -8540,16 +8655,16 @@
       <c r="G10" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H10" s="30" t="s">
-        <v>803</v>
-      </c>
-      <c r="I10" s="30"/>
+      <c r="H10" s="32" t="s">
+        <v>815</v>
+      </c>
+      <c r="I10" s="32"/>
       <c r="J10" s="122" t="s">
         <v>790</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="27" customFormat="1" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="124"/>
+    <row r="11" spans="1:10" s="27" customFormat="1" ht="78.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="126"/>
       <c r="B11" s="49" t="s">
         <v>205</v>
       </c>
@@ -8568,14 +8683,16 @@
       <c r="G11" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="30"/>
-      <c r="I11" s="30"/>
+      <c r="H11" s="32" t="s">
+        <v>816</v>
+      </c>
+      <c r="I11" s="32"/>
       <c r="J11" s="122" t="s">
         <v>790</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="27" customFormat="1" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="124"/>
+    <row r="12" spans="1:10" s="27" customFormat="1" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="126"/>
       <c r="B12" s="49" t="s">
         <v>207</v>
       </c>
@@ -8594,16 +8711,16 @@
       <c r="G12" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H12" s="30" t="s">
-        <v>804</v>
-      </c>
-      <c r="I12" s="30"/>
+      <c r="H12" s="32" t="s">
+        <v>817</v>
+      </c>
+      <c r="I12" s="32"/>
       <c r="J12" s="34" t="s">
         <v>792</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="27" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="124"/>
+    <row r="13" spans="1:10" s="27" customFormat="1" ht="141" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="126"/>
       <c r="B13" s="49" t="s">
         <v>209</v>
       </c>
@@ -8622,16 +8739,16 @@
       <c r="G13" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H13" s="30" t="s">
-        <v>805</v>
-      </c>
-      <c r="I13" s="30"/>
+      <c r="H13" s="32" t="s">
+        <v>818</v>
+      </c>
+      <c r="I13" s="32"/>
       <c r="J13" s="34" t="s">
         <v>792</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="27" customFormat="1" ht="111" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="124" t="s">
+    <row r="14" spans="1:10" s="27" customFormat="1" ht="111" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="126" t="s">
         <v>211</v>
       </c>
       <c r="B14" s="49" t="s">
@@ -8652,12 +8769,14 @@
       <c r="G14" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="H14" s="30"/>
-      <c r="I14" s="30"/>
+      <c r="H14" s="128"/>
+      <c r="I14" s="32" t="s">
+        <v>830</v>
+      </c>
       <c r="J14" s="34"/>
     </row>
-    <row r="15" spans="1:10" s="27" customFormat="1" ht="78" x14ac:dyDescent="0.3">
-      <c r="A15" s="124"/>
+    <row r="15" spans="1:10" s="27" customFormat="1" ht="94.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="126"/>
       <c r="B15" s="49" t="s">
         <v>215</v>
       </c>
@@ -8676,12 +8795,14 @@
       <c r="G15" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="H15" s="30"/>
-      <c r="I15" s="30"/>
+      <c r="H15" s="128"/>
+      <c r="I15" s="32" t="s">
+        <v>831</v>
+      </c>
       <c r="J15" s="34"/>
     </row>
-    <row r="16" spans="1:10" s="27" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="124"/>
+    <row r="16" spans="1:10" s="27" customFormat="1" ht="94.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="126"/>
       <c r="B16" s="49" t="s">
         <v>218</v>
       </c>
@@ -8698,12 +8819,14 @@
       <c r="G16" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="H16" s="30"/>
-      <c r="I16" s="30"/>
+      <c r="H16" s="128"/>
+      <c r="I16" s="32" t="s">
+        <v>831</v>
+      </c>
       <c r="J16" s="34"/>
     </row>
-    <row r="17" spans="1:10" s="27" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="124"/>
+    <row r="17" spans="1:10" s="27" customFormat="1" ht="125.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="126"/>
       <c r="B17" s="49" t="s">
         <v>220</v>
       </c>
@@ -8722,14 +8845,16 @@
       <c r="G17" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
+      <c r="H17" s="32" t="s">
+        <v>819</v>
+      </c>
+      <c r="I17" s="32"/>
       <c r="J17" s="34" t="s">
         <v>793</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="27" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="124"/>
+    <row r="18" spans="1:10" s="27" customFormat="1" ht="63" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="126"/>
       <c r="B18" s="49" t="s">
         <v>223</v>
       </c>
@@ -8748,12 +8873,14 @@
       <c r="G18" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="H18" s="30"/>
-      <c r="I18" s="30"/>
+      <c r="H18" s="128"/>
+      <c r="I18" s="32" t="s">
+        <v>832</v>
+      </c>
       <c r="J18" s="34"/>
     </row>
-    <row r="19" spans="1:10" s="27" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="124"/>
+    <row r="19" spans="1:10" s="27" customFormat="1" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="126"/>
       <c r="B19" s="49" t="s">
         <v>226</v>
       </c>
@@ -8772,12 +8899,14 @@
       <c r="G19" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="H19" s="30"/>
-      <c r="I19" s="30"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="32" t="s">
+        <v>833</v>
+      </c>
       <c r="J19" s="34"/>
     </row>
-    <row r="20" spans="1:10" s="27" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="124"/>
+    <row r="20" spans="1:10" s="27" customFormat="1" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="126"/>
       <c r="B20" s="49" t="s">
         <v>229</v>
       </c>
@@ -8796,12 +8925,14 @@
       <c r="G20" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="H20" s="30"/>
-      <c r="I20" s="30"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32" t="s">
+        <v>833</v>
+      </c>
       <c r="J20" s="34"/>
     </row>
-    <row r="21" spans="1:10" s="27" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="124" t="s">
+    <row r="21" spans="1:10" s="27" customFormat="1" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="126" t="s">
         <v>232</v>
       </c>
       <c r="B21" s="49" t="s">
@@ -8820,16 +8951,18 @@
         <v>235</v>
       </c>
       <c r="G21" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="H21" s="30"/>
-      <c r="I21" s="30"/>
+        <v>61</v>
+      </c>
+      <c r="H21" s="32"/>
+      <c r="I21" s="32" t="s">
+        <v>820</v>
+      </c>
       <c r="J21" s="34" t="s">
         <v>794</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="27" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="124"/>
+    <row r="22" spans="1:10" s="27" customFormat="1" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="126"/>
       <c r="B22" s="49" t="s">
         <v>236</v>
       </c>
@@ -8848,12 +8981,14 @@
       <c r="G22" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="H22" s="30"/>
-      <c r="I22" s="30"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="32" t="s">
+        <v>834</v>
+      </c>
       <c r="J22" s="34"/>
     </row>
-    <row r="23" spans="1:10" s="27" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A23" s="124"/>
+    <row r="23" spans="1:10" s="27" customFormat="1" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="126"/>
       <c r="B23" s="49" t="s">
         <v>239</v>
       </c>
@@ -8872,12 +9007,14 @@
       <c r="G23" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="H23" s="30"/>
-      <c r="I23" s="30"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="32" t="s">
+        <v>835</v>
+      </c>
       <c r="J23" s="34"/>
     </row>
-    <row r="24" spans="1:10" s="27" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="124" t="s">
+    <row r="24" spans="1:10" s="27" customFormat="1" ht="95.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="126" t="s">
         <v>242</v>
       </c>
       <c r="B24" s="49" t="s">
@@ -8898,14 +9035,16 @@
       <c r="G24" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H24" s="30"/>
-      <c r="I24" s="30"/>
+      <c r="H24" s="32" t="s">
+        <v>821</v>
+      </c>
+      <c r="I24" s="32"/>
       <c r="J24" s="34" t="s">
         <v>791</v>
       </c>
     </row>
-    <row r="25" spans="1:10" s="27" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A25" s="124"/>
+    <row r="25" spans="1:10" s="27" customFormat="1" ht="63" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="126"/>
       <c r="B25" s="49" t="s">
         <v>245</v>
       </c>
@@ -8924,14 +9063,16 @@
       <c r="G25" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H25" s="30"/>
-      <c r="I25" s="30"/>
+      <c r="H25" s="32" t="s">
+        <v>822</v>
+      </c>
+      <c r="I25" s="32"/>
       <c r="J25" s="34" t="s">
         <v>791</v>
       </c>
     </row>
-    <row r="26" spans="1:10" s="27" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A26" s="124"/>
+    <row r="26" spans="1:10" s="27" customFormat="1" ht="63" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="126"/>
       <c r="B26" s="49" t="s">
         <v>247</v>
       </c>
@@ -8950,12 +9091,12 @@
       <c r="G26" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="H26" s="30"/>
-      <c r="I26" s="30"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
       <c r="J26" s="34"/>
     </row>
-    <row r="27" spans="1:10" s="27" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="124"/>
+    <row r="27" spans="1:10" s="27" customFormat="1" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="126"/>
       <c r="B27" s="49" t="s">
         <v>249</v>
       </c>
@@ -8974,14 +9115,16 @@
       <c r="G27" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H27" s="30"/>
-      <c r="I27" s="30"/>
+      <c r="H27" s="32" t="s">
+        <v>823</v>
+      </c>
+      <c r="I27" s="32"/>
       <c r="J27" s="34" t="s">
         <v>791</v>
       </c>
     </row>
-    <row r="28" spans="1:10" s="27" customFormat="1" ht="109.2" x14ac:dyDescent="0.3">
-      <c r="A28" s="124"/>
+    <row r="28" spans="1:10" s="27" customFormat="1" ht="109.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="126"/>
       <c r="B28" s="49" t="s">
         <v>251</v>
       </c>
@@ -9000,12 +9143,14 @@
       <c r="G28" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="H28" s="30"/>
-      <c r="I28" s="30"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32" t="s">
+        <v>846</v>
+      </c>
       <c r="J28" s="34"/>
     </row>
-    <row r="29" spans="1:10" s="27" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="124" t="s">
+    <row r="29" spans="1:10" s="27" customFormat="1" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="126" t="s">
         <v>253</v>
       </c>
       <c r="B29" s="49" t="s">
@@ -9026,12 +9171,14 @@
       <c r="G29" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H29" s="30"/>
-      <c r="I29" s="30"/>
+      <c r="H29" s="32" t="s">
+        <v>848</v>
+      </c>
+      <c r="I29" s="32"/>
       <c r="J29" s="34"/>
     </row>
-    <row r="30" spans="1:10" s="27" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A30" s="124"/>
+    <row r="30" spans="1:10" s="27" customFormat="1" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="126"/>
       <c r="B30" s="49" t="s">
         <v>256</v>
       </c>
@@ -9050,14 +9197,16 @@
       <c r="G30" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H30" s="30"/>
-      <c r="I30" s="30"/>
+      <c r="H30" s="32" t="s">
+        <v>836</v>
+      </c>
+      <c r="I30" s="32"/>
       <c r="J30" s="34" t="s">
         <v>795</v>
       </c>
     </row>
-    <row r="31" spans="1:10" s="27" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="124"/>
+    <row r="31" spans="1:10" s="27" customFormat="1" ht="78.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="126"/>
       <c r="B31" s="49" t="s">
         <v>258</v>
       </c>
@@ -9076,14 +9225,16 @@
       <c r="G31" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H31" s="30"/>
-      <c r="I31" s="30"/>
+      <c r="H31" s="32" t="s">
+        <v>837</v>
+      </c>
+      <c r="I31" s="32"/>
       <c r="J31" s="34" t="s">
         <v>795</v>
       </c>
     </row>
-    <row r="32" spans="1:10" s="27" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A32" s="124"/>
+    <row r="32" spans="1:10" s="27" customFormat="1" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="126"/>
       <c r="B32" s="49" t="s">
         <v>260</v>
       </c>
@@ -9102,14 +9253,14 @@
       <c r="G32" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H32" s="30"/>
-      <c r="I32" s="30"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="32"/>
       <c r="J32" s="34" t="s">
         <v>791</v>
       </c>
     </row>
-    <row r="33" spans="1:10" s="27" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A33" s="124"/>
+    <row r="33" spans="1:10" s="27" customFormat="1" ht="63" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="126"/>
       <c r="B33" s="49" t="s">
         <v>262</v>
       </c>
@@ -9126,14 +9277,16 @@
         <v>264</v>
       </c>
       <c r="G33" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="H33" s="30"/>
-      <c r="I33" s="30"/>
+        <v>61</v>
+      </c>
+      <c r="H33" s="32"/>
+      <c r="I33" s="32" t="s">
+        <v>847</v>
+      </c>
       <c r="J33" s="34"/>
     </row>
-    <row r="34" spans="1:10" s="27" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A34" s="124"/>
+    <row r="34" spans="1:10" s="27" customFormat="1" ht="63" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="126"/>
       <c r="B34" s="49" t="s">
         <v>265</v>
       </c>
@@ -9152,12 +9305,14 @@
       <c r="G34" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="H34" s="30"/>
-      <c r="I34" s="30"/>
+      <c r="H34" s="32"/>
+      <c r="I34" s="32" t="s">
+        <v>838</v>
+      </c>
       <c r="J34" s="34"/>
     </row>
-    <row r="35" spans="1:10" s="27" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A35" s="124"/>
+    <row r="35" spans="1:10" s="27" customFormat="1" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="126"/>
       <c r="B35" s="49" t="s">
         <v>267</v>
       </c>
@@ -9176,12 +9331,14 @@
       <c r="G35" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="H35" s="30"/>
-      <c r="I35" s="30"/>
+      <c r="H35" s="32"/>
+      <c r="I35" s="32" t="s">
+        <v>838</v>
+      </c>
       <c r="J35" s="34"/>
     </row>
-    <row r="36" spans="1:10" s="27" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="124" t="s">
+    <row r="36" spans="1:10" s="27" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="126" t="s">
         <v>269</v>
       </c>
       <c r="B36" s="49" t="s">
@@ -9202,12 +9359,14 @@
       <c r="G36" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="H36" s="30"/>
-      <c r="I36" s="30"/>
+      <c r="H36" s="32"/>
+      <c r="I36" s="32" t="s">
+        <v>844</v>
+      </c>
       <c r="J36" s="34"/>
     </row>
-    <row r="37" spans="1:10" s="27" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="124"/>
+    <row r="37" spans="1:10" s="27" customFormat="1" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="126"/>
       <c r="B37" s="49" t="s">
         <v>273</v>
       </c>
@@ -9226,12 +9385,14 @@
       <c r="G37" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="H37" s="30"/>
-      <c r="I37" s="30"/>
+      <c r="H37" s="32"/>
+      <c r="I37" s="32" t="s">
+        <v>844</v>
+      </c>
       <c r="J37" s="34"/>
     </row>
-    <row r="38" spans="1:10" s="27" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A38" s="124"/>
+    <row r="38" spans="1:10" s="27" customFormat="1" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="126"/>
       <c r="B38" s="49" t="s">
         <v>275</v>
       </c>
@@ -9250,12 +9411,14 @@
       <c r="G38" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="H38" s="30"/>
-      <c r="I38" s="30"/>
+      <c r="H38" s="32"/>
+      <c r="I38" s="32" t="s">
+        <v>844</v>
+      </c>
       <c r="J38" s="34"/>
     </row>
-    <row r="39" spans="1:10" s="27" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="124" t="s">
+    <row r="39" spans="1:10" s="27" customFormat="1" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="126" t="s">
         <v>277</v>
       </c>
       <c r="B39" s="49" t="s">
@@ -9276,12 +9439,14 @@
       <c r="G39" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="H39" s="30"/>
-      <c r="I39" s="30"/>
+      <c r="H39" s="32"/>
+      <c r="I39" s="32" t="s">
+        <v>845</v>
+      </c>
       <c r="J39" s="34"/>
     </row>
-    <row r="40" spans="1:10" s="27" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A40" s="124"/>
+    <row r="40" spans="1:10" s="27" customFormat="1" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="126"/>
       <c r="B40" s="49" t="s">
         <v>281</v>
       </c>
@@ -9300,12 +9465,14 @@
       <c r="G40" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="H40" s="30"/>
-      <c r="I40" s="30"/>
+      <c r="H40" s="32"/>
+      <c r="I40" s="32" t="s">
+        <v>846</v>
+      </c>
       <c r="J40" s="34"/>
     </row>
-    <row r="41" spans="1:10" s="27" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A41" s="124"/>
+    <row r="41" spans="1:10" s="27" customFormat="1" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="126"/>
       <c r="B41" s="49" t="s">
         <v>283</v>
       </c>
@@ -9324,12 +9491,14 @@
       <c r="G41" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="H41" s="30"/>
-      <c r="I41" s="30"/>
+      <c r="H41" s="32"/>
+      <c r="I41" s="32" t="s">
+        <v>846</v>
+      </c>
       <c r="J41" s="34"/>
     </row>
-    <row r="42" spans="1:10" s="27" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A42" s="124"/>
+    <row r="42" spans="1:10" s="27" customFormat="1" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="126"/>
       <c r="B42" s="49" t="s">
         <v>285</v>
       </c>
@@ -9348,12 +9517,14 @@
       <c r="G42" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="H42" s="30"/>
-      <c r="I42" s="30"/>
+      <c r="H42" s="32"/>
+      <c r="I42" s="32" t="s">
+        <v>846</v>
+      </c>
       <c r="J42" s="34"/>
     </row>
-    <row r="43" spans="1:10" s="27" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A43" s="124"/>
+    <row r="43" spans="1:10" s="27" customFormat="1" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="126"/>
       <c r="B43" s="49" t="s">
         <v>287</v>
       </c>
@@ -9372,12 +9543,14 @@
       <c r="G43" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="H43" s="30"/>
-      <c r="I43" s="30"/>
+      <c r="H43" s="32"/>
+      <c r="I43" s="32" t="s">
+        <v>846</v>
+      </c>
       <c r="J43" s="34"/>
     </row>
-    <row r="44" spans="1:10" s="27" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A44" s="124"/>
+    <row r="44" spans="1:10" s="27" customFormat="1" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="126"/>
       <c r="B44" s="49" t="s">
         <v>289</v>
       </c>
@@ -9396,12 +9569,14 @@
       <c r="G44" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="H44" s="30"/>
-      <c r="I44" s="30"/>
+      <c r="H44" s="32"/>
+      <c r="I44" s="32" t="s">
+        <v>846</v>
+      </c>
       <c r="J44" s="34"/>
     </row>
-    <row r="45" spans="1:10" s="27" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="124" t="s">
+    <row r="45" spans="1:10" s="27" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="126" t="s">
         <v>291</v>
       </c>
       <c r="B45" s="49" t="s">
@@ -9422,14 +9597,16 @@
       <c r="G45" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H45" s="30"/>
-      <c r="I45" s="30"/>
+      <c r="H45" s="32" t="s">
+        <v>824</v>
+      </c>
+      <c r="I45" s="32"/>
       <c r="J45" s="34" t="s">
         <v>790</v>
       </c>
     </row>
-    <row r="46" spans="1:10" s="27" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A46" s="124"/>
+    <row r="46" spans="1:10" s="27" customFormat="1" ht="63" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="126"/>
       <c r="B46" s="49" t="s">
         <v>295</v>
       </c>
@@ -9448,14 +9625,16 @@
       <c r="G46" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H46" s="30"/>
-      <c r="I46" s="30"/>
+      <c r="H46" s="32" t="s">
+        <v>825</v>
+      </c>
+      <c r="I46" s="32"/>
       <c r="J46" s="34" t="s">
         <v>791</v>
       </c>
     </row>
-    <row r="47" spans="1:10" s="27" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A47" s="124"/>
+    <row r="47" spans="1:10" s="27" customFormat="1" ht="63" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="126"/>
       <c r="B47" s="49" t="s">
         <v>297</v>
       </c>
@@ -9474,14 +9653,16 @@
       <c r="G47" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H47" s="30"/>
-      <c r="I47" s="30"/>
+      <c r="H47" s="32" t="s">
+        <v>826</v>
+      </c>
+      <c r="I47" s="32"/>
       <c r="J47" s="34" t="s">
         <v>791</v>
       </c>
     </row>
-    <row r="48" spans="1:10" s="27" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A48" s="124"/>
+    <row r="48" spans="1:10" s="27" customFormat="1" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="126"/>
       <c r="B48" s="49" t="s">
         <v>299</v>
       </c>
@@ -9500,14 +9681,16 @@
       <c r="G48" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H48" s="30"/>
-      <c r="I48" s="30"/>
+      <c r="H48" s="32" t="s">
+        <v>827</v>
+      </c>
+      <c r="I48" s="32"/>
       <c r="J48" s="34" t="s">
         <v>791</v>
       </c>
     </row>
-    <row r="49" spans="1:10" s="27" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A49" s="124"/>
+    <row r="49" spans="1:10" s="27" customFormat="1" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="126"/>
       <c r="B49" s="49" t="s">
         <v>301</v>
       </c>
@@ -9526,12 +9709,14 @@
       <c r="G49" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="H49" s="30"/>
-      <c r="I49" s="30"/>
+      <c r="H49" s="32"/>
+      <c r="I49" s="32" t="s">
+        <v>838</v>
+      </c>
       <c r="J49" s="34"/>
     </row>
-    <row r="50" spans="1:10" s="27" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A50" s="124"/>
+    <row r="50" spans="1:10" s="27" customFormat="1" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="126"/>
       <c r="B50" s="49" t="s">
         <v>304</v>
       </c>
@@ -9550,12 +9735,14 @@
       <c r="G50" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="H50" s="30"/>
-      <c r="I50" s="30"/>
+      <c r="H50" s="32"/>
+      <c r="I50" s="32" t="s">
+        <v>838</v>
+      </c>
       <c r="J50" s="34"/>
     </row>
-    <row r="51" spans="1:10" s="27" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A51" s="124"/>
+    <row r="51" spans="1:10" s="27" customFormat="1" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="126"/>
       <c r="B51" s="49" t="s">
         <v>307</v>
       </c>
@@ -9572,14 +9759,16 @@
         <v>309</v>
       </c>
       <c r="G51" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="H51" s="30"/>
-      <c r="I51" s="30"/>
+        <v>61</v>
+      </c>
+      <c r="H51" s="128"/>
+      <c r="I51" s="32" t="s">
+        <v>828</v>
+      </c>
       <c r="J51" s="34"/>
     </row>
-    <row r="52" spans="1:10" s="27" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="124" t="s">
+    <row r="52" spans="1:10" s="27" customFormat="1" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="126" t="s">
         <v>310</v>
       </c>
       <c r="B52" s="49" t="s">
@@ -9600,12 +9789,14 @@
       <c r="G52" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="H52" s="30"/>
-      <c r="I52" s="30"/>
+      <c r="H52" s="32"/>
+      <c r="I52" s="32" t="s">
+        <v>843</v>
+      </c>
       <c r="J52" s="34"/>
     </row>
-    <row r="53" spans="1:10" s="27" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A53" s="124"/>
+    <row r="53" spans="1:10" s="27" customFormat="1" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="126"/>
       <c r="B53" s="49" t="s">
         <v>314</v>
       </c>
@@ -9624,12 +9815,14 @@
       <c r="G53" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="H53" s="30"/>
-      <c r="I53" s="30"/>
+      <c r="H53" s="32"/>
+      <c r="I53" s="32" t="s">
+        <v>842</v>
+      </c>
       <c r="J53" s="34"/>
     </row>
-    <row r="54" spans="1:10" s="27" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A54" s="124"/>
+    <row r="54" spans="1:10" s="27" customFormat="1" ht="63" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="126"/>
       <c r="B54" s="49" t="s">
         <v>316</v>
       </c>
@@ -9648,14 +9841,16 @@
       <c r="G54" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H54" s="30"/>
-      <c r="I54" s="30"/>
+      <c r="H54" s="32" t="s">
+        <v>826</v>
+      </c>
+      <c r="I54" s="32"/>
       <c r="J54" s="34" t="s">
         <v>791</v>
       </c>
     </row>
-    <row r="55" spans="1:10" s="27" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="124" t="s">
+    <row r="55" spans="1:10" s="27" customFormat="1" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="126" t="s">
         <v>318</v>
       </c>
       <c r="B55" s="49" t="s">
@@ -9676,14 +9871,14 @@
       <c r="G55" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H55" s="30"/>
-      <c r="I55" s="30"/>
+      <c r="H55" s="32"/>
+      <c r="I55" s="32"/>
       <c r="J55" s="34" t="s">
         <v>791</v>
       </c>
     </row>
-    <row r="56" spans="1:10" s="27" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A56" s="124"/>
+    <row r="56" spans="1:10" s="27" customFormat="1" ht="78.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="126"/>
       <c r="B56" s="49" t="s">
         <v>323</v>
       </c>
@@ -9702,14 +9897,16 @@
       <c r="G56" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H56" s="30"/>
-      <c r="I56" s="30"/>
+      <c r="H56" s="32" t="s">
+        <v>841</v>
+      </c>
+      <c r="I56" s="32"/>
       <c r="J56" s="34" t="s">
         <v>791</v>
       </c>
     </row>
-    <row r="57" spans="1:10" s="27" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A57" s="124"/>
+    <row r="57" spans="1:10" s="27" customFormat="1" ht="78.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="126"/>
       <c r="B57" s="49" t="s">
         <v>325</v>
       </c>
@@ -9728,14 +9925,16 @@
       <c r="G57" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H57" s="30"/>
-      <c r="I57" s="30"/>
+      <c r="H57" s="32" t="s">
+        <v>840</v>
+      </c>
+      <c r="I57" s="32"/>
       <c r="J57" s="34" t="s">
         <v>791</v>
       </c>
     </row>
-    <row r="58" spans="1:10" s="27" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A58" s="124"/>
+    <row r="58" spans="1:10" s="27" customFormat="1" ht="94.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="126"/>
       <c r="B58" s="49" t="s">
         <v>327</v>
       </c>
@@ -9752,24 +9951,26 @@
       <c r="G58" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="H58" s="40"/>
-      <c r="I58" s="40"/>
+      <c r="H58" s="129" t="s">
+        <v>839</v>
+      </c>
+      <c r="I58" s="129"/>
       <c r="J58" s="43" t="s">
         <v>791</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="A39:A44"/>
+    <mergeCell ref="A45:A51"/>
+    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="A55:A58"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="A14:A20"/>
     <mergeCell ref="A21:A23"/>
     <mergeCell ref="A24:A28"/>
     <mergeCell ref="A29:A35"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="A39:A44"/>
-    <mergeCell ref="A45:A51"/>
-    <mergeCell ref="A52:A54"/>
-    <mergeCell ref="A55:A58"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="G2:G58" xr:uid="{00000000-0002-0000-0200-000000000000}">
@@ -9865,7 +10066,7 @@
       <c r="J2" s="55"/>
     </row>
     <row r="3" spans="1:10" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="124" t="s">
+      <c r="A3" s="126" t="s">
         <v>332</v>
       </c>
       <c r="B3" s="68" t="s">
@@ -9891,7 +10092,7 @@
       <c r="J3" s="34"/>
     </row>
     <row r="4" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="124"/>
+      <c r="A4" s="126"/>
       <c r="B4" s="68" t="s">
         <v>335</v>
       </c>
@@ -9915,7 +10116,7 @@
       <c r="J4" s="34"/>
     </row>
     <row r="5" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="124"/>
+      <c r="A5" s="126"/>
       <c r="B5" s="68" t="s">
         <v>337</v>
       </c>
@@ -9939,7 +10140,7 @@
       <c r="J5" s="34"/>
     </row>
     <row r="6" spans="1:10" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="124"/>
+      <c r="A6" s="126"/>
       <c r="B6" s="68" t="s">
         <v>339</v>
       </c>
@@ -9963,7 +10164,7 @@
       <c r="J6" s="34"/>
     </row>
     <row r="7" spans="1:10" ht="79.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="124" t="s">
+      <c r="A7" s="126" t="s">
         <v>341</v>
       </c>
       <c r="B7" s="68" t="s">
@@ -9989,7 +10190,7 @@
       <c r="J7" s="34"/>
     </row>
     <row r="8" spans="1:10" ht="109.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="124"/>
+      <c r="A8" s="126"/>
       <c r="B8" s="68" t="s">
         <v>344</v>
       </c>
@@ -10013,7 +10214,7 @@
       <c r="J8" s="34"/>
     </row>
     <row r="9" spans="1:10" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="124"/>
+      <c r="A9" s="126"/>
       <c r="B9" s="68" t="s">
         <v>346</v>
       </c>
@@ -10035,7 +10236,7 @@
       <c r="J9" s="34"/>
     </row>
     <row r="10" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="124"/>
+      <c r="A10" s="126"/>
       <c r="B10" s="68" t="s">
         <v>348</v>
       </c>
@@ -10059,7 +10260,7 @@
       <c r="J10" s="34"/>
     </row>
     <row r="11" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="124" t="s">
+      <c r="A11" s="126" t="s">
         <v>350</v>
       </c>
       <c r="B11" s="68" t="s">
@@ -10085,7 +10286,7 @@
       <c r="J11" s="34"/>
     </row>
     <row r="12" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="124"/>
+      <c r="A12" s="126"/>
       <c r="B12" s="68" t="s">
         <v>354</v>
       </c>
@@ -10109,7 +10310,7 @@
       <c r="J12" s="34"/>
     </row>
     <row r="13" spans="1:10" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="124"/>
+      <c r="A13" s="126"/>
       <c r="B13" s="68" t="s">
         <v>356</v>
       </c>
@@ -10133,7 +10334,7 @@
       <c r="J13" s="34"/>
     </row>
     <row r="14" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="124"/>
+      <c r="A14" s="126"/>
       <c r="B14" s="68" t="s">
         <v>358</v>
       </c>
@@ -10157,7 +10358,7 @@
       <c r="J14" s="34"/>
     </row>
     <row r="15" spans="1:10" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="124"/>
+      <c r="A15" s="126"/>
       <c r="B15" s="68" t="s">
         <v>360</v>
       </c>
@@ -10181,7 +10382,7 @@
       <c r="J15" s="34"/>
     </row>
     <row r="16" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="124" t="s">
+      <c r="A16" s="126" t="s">
         <v>362</v>
       </c>
       <c r="B16" s="68" t="s">
@@ -10207,7 +10408,7 @@
       <c r="J16" s="34"/>
     </row>
     <row r="17" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="124"/>
+      <c r="A17" s="126"/>
       <c r="B17" s="68" t="s">
         <v>366</v>
       </c>
@@ -10229,7 +10430,7 @@
       <c r="J17" s="34"/>
     </row>
     <row r="18" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="124"/>
+      <c r="A18" s="126"/>
       <c r="B18" s="68" t="s">
         <v>368</v>
       </c>
@@ -10251,7 +10452,7 @@
       <c r="J18" s="34"/>
     </row>
     <row r="19" spans="1:10" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="124" t="s">
+      <c r="A19" s="126" t="s">
         <v>370</v>
       </c>
       <c r="B19" s="68" t="s">
@@ -10277,7 +10478,7 @@
       <c r="J19" s="34"/>
     </row>
     <row r="20" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="124"/>
+      <c r="A20" s="126"/>
       <c r="B20" s="68" t="s">
         <v>374</v>
       </c>
@@ -10411,7 +10612,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="124" t="s">
+      <c r="A2" s="126" t="s">
         <v>379</v>
       </c>
       <c r="B2" s="76" t="s">
@@ -10435,7 +10636,7 @@
       <c r="J2" s="55"/>
     </row>
     <row r="3" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="124"/>
+      <c r="A3" s="126"/>
       <c r="B3" s="76" t="s">
         <v>382</v>
       </c>
@@ -10457,7 +10658,7 @@
       <c r="J3" s="34"/>
     </row>
     <row r="4" spans="1:10" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="124"/>
+      <c r="A4" s="126"/>
       <c r="B4" s="76" t="s">
         <v>384</v>
       </c>
@@ -10479,7 +10680,7 @@
       <c r="J4" s="34"/>
     </row>
     <row r="5" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="124"/>
+      <c r="A5" s="126"/>
       <c r="B5" s="76" t="s">
         <v>386</v>
       </c>
@@ -10501,7 +10702,7 @@
       <c r="J5" s="34"/>
     </row>
     <row r="6" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="124"/>
+      <c r="A6" s="126"/>
       <c r="B6" s="76" t="s">
         <v>387</v>
       </c>
@@ -10523,7 +10724,7 @@
       <c r="J6" s="34"/>
     </row>
     <row r="7" spans="1:10" ht="79.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="124" t="s">
+      <c r="A7" s="126" t="s">
         <v>389</v>
       </c>
       <c r="B7" s="76" t="s">
@@ -10547,7 +10748,7 @@
       <c r="J7" s="34"/>
     </row>
     <row r="8" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="124"/>
+      <c r="A8" s="126"/>
       <c r="B8" s="76" t="s">
         <v>392</v>
       </c>
@@ -10569,7 +10770,7 @@
       <c r="J8" s="34"/>
     </row>
     <row r="9" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="124" t="s">
+      <c r="A9" s="126" t="s">
         <v>394</v>
       </c>
       <c r="B9" s="76" t="s">
@@ -10593,7 +10794,7 @@
       <c r="J9" s="34"/>
     </row>
     <row r="10" spans="1:10" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="124"/>
+      <c r="A10" s="126"/>
       <c r="B10" s="76" t="s">
         <v>397</v>
       </c>
@@ -10615,7 +10816,7 @@
       <c r="J10" s="34"/>
     </row>
     <row r="11" spans="1:10" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="124"/>
+      <c r="A11" s="126"/>
       <c r="B11" s="76" t="s">
         <v>399</v>
       </c>
@@ -10711,7 +10912,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="79.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="124" t="s">
+      <c r="A2" s="126" t="s">
         <v>401</v>
       </c>
       <c r="B2" s="68" t="s">
@@ -10735,7 +10936,7 @@
       <c r="J2" s="55"/>
     </row>
     <row r="3" spans="1:10" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="124"/>
+      <c r="A3" s="126"/>
       <c r="B3" s="68" t="s">
         <v>404</v>
       </c>
@@ -10757,7 +10958,7 @@
       <c r="J3" s="34"/>
     </row>
     <row r="4" spans="1:10" ht="78" x14ac:dyDescent="0.3">
-      <c r="A4" s="124"/>
+      <c r="A4" s="126"/>
       <c r="B4" s="68" t="s">
         <v>406</v>
       </c>
@@ -10779,7 +10980,7 @@
       <c r="J4" s="34"/>
     </row>
     <row r="5" spans="1:10" ht="109.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="124"/>
+      <c r="A5" s="126"/>
       <c r="B5" s="68" t="s">
         <v>408</v>
       </c>
@@ -10801,7 +11002,7 @@
       <c r="J5" s="34"/>
     </row>
     <row r="6" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="124"/>
+      <c r="A6" s="126"/>
       <c r="B6" s="68" t="s">
         <v>410</v>
       </c>
@@ -10823,7 +11024,7 @@
       <c r="J6" s="34"/>
     </row>
     <row r="7" spans="1:10" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="124" t="s">
+      <c r="A7" s="126" t="s">
         <v>412</v>
       </c>
       <c r="B7" s="68" t="s">
@@ -10847,7 +11048,7 @@
       <c r="J7" s="34"/>
     </row>
     <row r="8" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="124"/>
+      <c r="A8" s="126"/>
       <c r="B8" s="68" t="s">
         <v>414</v>
       </c>
@@ -10869,7 +11070,7 @@
       <c r="J8" s="34"/>
     </row>
     <row r="9" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="124"/>
+      <c r="A9" s="126"/>
       <c r="B9" s="68" t="s">
         <v>308</v>
       </c>
@@ -10891,7 +11092,7 @@
       <c r="J9" s="34"/>
     </row>
     <row r="10" spans="1:10" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="124"/>
+      <c r="A10" s="126"/>
       <c r="B10" s="68" t="s">
         <v>417</v>
       </c>
@@ -10913,7 +11114,7 @@
       <c r="J10" s="34"/>
     </row>
     <row r="11" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="124"/>
+      <c r="A11" s="126"/>
       <c r="B11" s="68" t="s">
         <v>221</v>
       </c>
@@ -10935,7 +11136,7 @@
       <c r="J11" s="34"/>
     </row>
     <row r="12" spans="1:10" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="124"/>
+      <c r="A12" s="126"/>
       <c r="B12" s="68" t="s">
         <v>224</v>
       </c>
@@ -10957,7 +11158,7 @@
       <c r="J12" s="34"/>
     </row>
     <row r="13" spans="1:10" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="124"/>
+      <c r="A13" s="126"/>
       <c r="B13" s="68" t="s">
         <v>421</v>
       </c>
@@ -10979,7 +11180,7 @@
       <c r="J13" s="34"/>
     </row>
     <row r="14" spans="1:10" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="124"/>
+      <c r="A14" s="126"/>
       <c r="B14" s="68" t="s">
         <v>227</v>
       </c>
@@ -11001,7 +11202,7 @@
       <c r="J14" s="34"/>
     </row>
     <row r="15" spans="1:10" ht="126.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="124" t="s">
+      <c r="A15" s="126" t="s">
         <v>424</v>
       </c>
       <c r="B15" s="68" t="s">
@@ -11025,7 +11226,7 @@
       <c r="J15" s="34"/>
     </row>
     <row r="16" spans="1:10" ht="78" x14ac:dyDescent="0.3">
-      <c r="A16" s="124"/>
+      <c r="A16" s="126"/>
       <c r="B16" s="68" t="s">
         <v>427</v>
       </c>
@@ -11047,7 +11248,7 @@
       <c r="J16" s="34"/>
     </row>
     <row r="17" spans="1:10" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="124"/>
+      <c r="A17" s="126"/>
       <c r="B17" s="68" t="s">
         <v>429</v>
       </c>
@@ -11069,7 +11270,7 @@
       <c r="J17" s="34"/>
     </row>
     <row r="18" spans="1:10" ht="78" x14ac:dyDescent="0.3">
-      <c r="A18" s="124"/>
+      <c r="A18" s="126"/>
       <c r="B18" s="68" t="s">
         <v>431</v>
       </c>
@@ -11091,7 +11292,7 @@
       <c r="J18" s="34"/>
     </row>
     <row r="19" spans="1:10" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="124"/>
+      <c r="A19" s="126"/>
       <c r="B19" s="68" t="s">
         <v>433</v>
       </c>
@@ -11113,7 +11314,7 @@
       <c r="J19" s="34"/>
     </row>
     <row r="20" spans="1:10" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="124"/>
+      <c r="A20" s="126"/>
       <c r="B20" s="68" t="s">
         <v>435</v>
       </c>
@@ -11135,7 +11336,7 @@
       <c r="J20" s="34"/>
     </row>
     <row r="21" spans="1:10" ht="78" x14ac:dyDescent="0.3">
-      <c r="A21" s="124"/>
+      <c r="A21" s="126"/>
       <c r="B21" s="68" t="s">
         <v>437</v>
       </c>
@@ -11157,7 +11358,7 @@
       <c r="J21" s="34"/>
     </row>
     <row r="22" spans="1:10" ht="78" x14ac:dyDescent="0.3">
-      <c r="A22" s="124"/>
+      <c r="A22" s="126"/>
       <c r="B22" s="68" t="s">
         <v>439</v>
       </c>
@@ -11179,7 +11380,7 @@
       <c r="J22" s="34"/>
     </row>
     <row r="23" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A23" s="124"/>
+      <c r="A23" s="126"/>
       <c r="B23" s="68" t="s">
         <v>441</v>
       </c>
@@ -11201,7 +11402,7 @@
       <c r="J23" s="34"/>
     </row>
     <row r="24" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="124"/>
+      <c r="A24" s="126"/>
       <c r="B24" s="68" t="s">
         <v>443</v>
       </c>
@@ -11223,7 +11424,7 @@
       <c r="J24" s="34"/>
     </row>
     <row r="25" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="124" t="s">
+      <c r="A25" s="126" t="s">
         <v>445</v>
       </c>
       <c r="B25" s="68" t="s">
@@ -11247,7 +11448,7 @@
       <c r="J25" s="34"/>
     </row>
     <row r="26" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A26" s="124"/>
+      <c r="A26" s="126"/>
       <c r="B26" s="68" t="s">
         <v>448</v>
       </c>
@@ -11269,7 +11470,7 @@
       <c r="J26" s="34"/>
     </row>
     <row r="27" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A27" s="124"/>
+      <c r="A27" s="126"/>
       <c r="B27" s="68" t="s">
         <v>450</v>
       </c>
@@ -11291,7 +11492,7 @@
       <c r="J27" s="34"/>
     </row>
     <row r="28" spans="1:10" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="124" t="s">
+      <c r="A28" s="126" t="s">
         <v>452</v>
       </c>
       <c r="B28" s="68" t="s">
@@ -11315,7 +11516,7 @@
       <c r="J28" s="34"/>
     </row>
     <row r="29" spans="1:10" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A29" s="124"/>
+      <c r="A29" s="126"/>
       <c r="B29" s="68" t="s">
         <v>455</v>
       </c>
@@ -11337,7 +11538,7 @@
       <c r="J29" s="34"/>
     </row>
     <row r="30" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="124"/>
+      <c r="A30" s="126"/>
       <c r="B30" s="68" t="s">
         <v>457</v>
       </c>
@@ -11359,7 +11560,7 @@
       <c r="J30" s="34"/>
     </row>
     <row r="31" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="124"/>
+      <c r="A31" s="126"/>
       <c r="B31" s="68" t="s">
         <v>459</v>
       </c>
@@ -11458,7 +11659,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="124" t="s">
+      <c r="A2" s="126" t="s">
         <v>461</v>
       </c>
       <c r="B2" s="68" t="s">
@@ -11482,7 +11683,7 @@
       <c r="J2" s="55"/>
     </row>
     <row r="3" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="124"/>
+      <c r="A3" s="126"/>
       <c r="B3" s="68" t="s">
         <v>464</v>
       </c>
@@ -11504,7 +11705,7 @@
       <c r="J3" s="34"/>
     </row>
     <row r="4" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="124"/>
+      <c r="A4" s="126"/>
       <c r="B4" s="68" t="s">
         <v>237</v>
       </c>
@@ -11526,7 +11727,7 @@
       <c r="J4" s="34"/>
     </row>
     <row r="5" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="124" t="s">
+      <c r="A5" s="126" t="s">
         <v>467</v>
       </c>
       <c r="B5" s="68" t="s">
@@ -11550,7 +11751,7 @@
       <c r="J5" s="34"/>
     </row>
     <row r="6" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="124"/>
+      <c r="A6" s="126"/>
       <c r="B6" s="68" t="s">
         <v>470</v>
       </c>
@@ -11572,7 +11773,7 @@
       <c r="J6" s="34"/>
     </row>
     <row r="7" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="124"/>
+      <c r="A7" s="126"/>
       <c r="B7" s="68" t="s">
         <v>472</v>
       </c>
@@ -11594,7 +11795,7 @@
       <c r="J7" s="34"/>
     </row>
     <row r="8" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="124"/>
+      <c r="A8" s="126"/>
       <c r="B8" s="68" t="s">
         <v>474</v>
       </c>
@@ -11616,7 +11817,7 @@
       <c r="J8" s="34"/>
     </row>
     <row r="9" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="124"/>
+      <c r="A9" s="126"/>
       <c r="B9" s="68" t="s">
         <v>476</v>
       </c>
@@ -11638,7 +11839,7 @@
       <c r="J9" s="34"/>
     </row>
     <row r="10" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="124"/>
+      <c r="A10" s="126"/>
       <c r="B10" s="68" t="s">
         <v>478</v>
       </c>
@@ -11660,7 +11861,7 @@
       <c r="J10" s="34"/>
     </row>
     <row r="11" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="124"/>
+      <c r="A11" s="126"/>
       <c r="B11" s="68" t="s">
         <v>480</v>
       </c>
@@ -11682,7 +11883,7 @@
       <c r="J11" s="34"/>
     </row>
     <row r="12" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="124"/>
+      <c r="A12" s="126"/>
       <c r="B12" s="68" t="s">
         <v>482</v>
       </c>
@@ -11704,7 +11905,7 @@
       <c r="J12" s="34"/>
     </row>
     <row r="13" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="124" t="s">
+      <c r="A13" s="126" t="s">
         <v>484</v>
       </c>
       <c r="B13" s="68" t="s">
@@ -11728,7 +11929,7 @@
       <c r="J13" s="34"/>
     </row>
     <row r="14" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="124"/>
+      <c r="A14" s="126"/>
       <c r="B14" s="68" t="s">
         <v>487</v>
       </c>
@@ -11750,7 +11951,7 @@
       <c r="J14" s="34"/>
     </row>
     <row r="15" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="124"/>
+      <c r="A15" s="126"/>
       <c r="B15" s="68" t="s">
         <v>489</v>
       </c>
@@ -11772,7 +11973,7 @@
       <c r="J15" s="34"/>
     </row>
     <row r="16" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="124" t="s">
+      <c r="A16" s="126" t="s">
         <v>491</v>
       </c>
       <c r="B16" s="68" t="s">
@@ -11796,7 +11997,7 @@
       <c r="J16" s="34"/>
     </row>
     <row r="17" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="124"/>
+      <c r="A17" s="126"/>
       <c r="B17" s="68" t="s">
         <v>494</v>
       </c>
@@ -11894,7 +12095,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="124" t="s">
+      <c r="A2" s="126" t="s">
         <v>496</v>
       </c>
       <c r="B2" s="68" t="s">
@@ -11918,7 +12119,7 @@
       <c r="J2" s="91"/>
     </row>
     <row r="3" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="124"/>
+      <c r="A3" s="126"/>
       <c r="B3" s="68" t="s">
         <v>364</v>
       </c>
@@ -11940,7 +12141,7 @@
       <c r="J3" s="34"/>
     </row>
     <row r="4" spans="1:10" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="124"/>
+      <c r="A4" s="126"/>
       <c r="B4" s="68" t="s">
         <v>499</v>
       </c>
@@ -11962,7 +12163,7 @@
       <c r="J4" s="34"/>
     </row>
     <row r="5" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="124"/>
+      <c r="A5" s="126"/>
       <c r="B5" s="68" t="s">
         <v>501</v>
       </c>
@@ -11984,7 +12185,7 @@
       <c r="J5" s="34"/>
     </row>
     <row r="6" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="124" t="s">
+      <c r="A6" s="126" t="s">
         <v>503</v>
       </c>
       <c r="B6" s="68" t="s">
@@ -12008,7 +12209,7 @@
       <c r="J6" s="34"/>
     </row>
     <row r="7" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="124"/>
+      <c r="A7" s="126"/>
       <c r="B7" s="68" t="s">
         <v>505</v>
       </c>
@@ -12030,7 +12231,7 @@
       <c r="J7" s="34"/>
     </row>
     <row r="8" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="124" t="s">
+      <c r="A8" s="126" t="s">
         <v>507</v>
       </c>
       <c r="B8" s="68" t="s">
@@ -12054,7 +12255,7 @@
       <c r="J8" s="34"/>
     </row>
     <row r="9" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="124"/>
+      <c r="A9" s="126"/>
       <c r="B9" s="68" t="s">
         <v>510</v>
       </c>
@@ -12076,7 +12277,7 @@
       <c r="J9" s="34"/>
     </row>
     <row r="10" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="124"/>
+      <c r="A10" s="126"/>
       <c r="B10" s="68" t="s">
         <v>512</v>
       </c>
@@ -12098,7 +12299,7 @@
       <c r="J10" s="34"/>
     </row>
     <row r="11" spans="1:10" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="124"/>
+      <c r="A11" s="126"/>
       <c r="B11" s="68" t="s">
         <v>514</v>
       </c>
@@ -12118,7 +12319,7 @@
       <c r="J11" s="34"/>
     </row>
     <row r="12" spans="1:10" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="124" t="s">
+      <c r="A12" s="126" t="s">
         <v>516</v>
       </c>
       <c r="B12" s="68" t="s">
@@ -12142,7 +12343,7 @@
       <c r="J12" s="34"/>
     </row>
     <row r="13" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="124"/>
+      <c r="A13" s="126"/>
       <c r="B13" s="68" t="s">
         <v>519</v>
       </c>
@@ -12164,7 +12365,7 @@
       <c r="J13" s="34"/>
     </row>
     <row r="14" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="124"/>
+      <c r="A14" s="126"/>
       <c r="B14" s="68" t="s">
         <v>521</v>
       </c>
@@ -12261,7 +12462,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="124" t="s">
+      <c r="A2" s="126" t="s">
         <v>523</v>
       </c>
       <c r="B2" s="68" t="s">
@@ -12285,7 +12486,7 @@
       <c r="J2" s="55"/>
     </row>
     <row r="3" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="124"/>
+      <c r="A3" s="126"/>
       <c r="B3" s="68" t="s">
         <v>526</v>
       </c>
@@ -12307,7 +12508,7 @@
       <c r="J3" s="34"/>
     </row>
     <row r="4" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="124"/>
+      <c r="A4" s="126"/>
       <c r="B4" s="68" t="s">
         <v>528</v>
       </c>
@@ -12329,7 +12530,7 @@
       <c r="J4" s="34"/>
     </row>
     <row r="5" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="124"/>
+      <c r="A5" s="126"/>
       <c r="B5" s="68" t="s">
         <v>530</v>
       </c>
@@ -12351,7 +12552,7 @@
       <c r="J5" s="34"/>
     </row>
     <row r="6" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="124"/>
+      <c r="A6" s="126"/>
       <c r="B6" s="68" t="s">
         <v>532</v>
       </c>
@@ -12373,7 +12574,7 @@
       <c r="J6" s="34"/>
     </row>
     <row r="7" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="124"/>
+      <c r="A7" s="126"/>
       <c r="B7" s="68" t="s">
         <v>534</v>
       </c>
@@ -12395,7 +12596,7 @@
       <c r="J7" s="34"/>
     </row>
     <row r="8" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="124" t="s">
+      <c r="A8" s="126" t="s">
         <v>536</v>
       </c>
       <c r="B8" s="68" t="s">
@@ -12419,7 +12620,7 @@
       <c r="J8" s="34"/>
     </row>
     <row r="9" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="124"/>
+      <c r="A9" s="126"/>
       <c r="B9" s="68" t="s">
         <v>539</v>
       </c>
@@ -12441,7 +12642,7 @@
       <c r="J9" s="34"/>
     </row>
     <row r="10" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="124"/>
+      <c r="A10" s="126"/>
       <c r="B10" s="68" t="s">
         <v>541</v>
       </c>
@@ -12463,7 +12664,7 @@
       <c r="J10" s="34"/>
     </row>
     <row r="11" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="124" t="s">
+      <c r="A11" s="126" t="s">
         <v>543</v>
       </c>
       <c r="B11" s="68" t="s">
@@ -12487,7 +12688,7 @@
       <c r="J11" s="34"/>
     </row>
     <row r="12" spans="1:10" ht="93.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="124"/>
+      <c r="A12" s="126"/>
       <c r="B12" s="68" t="s">
         <v>546</v>
       </c>
@@ -12511,7 +12712,7 @@
       <c r="J12" s="34"/>
     </row>
     <row r="13" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="124"/>
+      <c r="A13" s="126"/>
       <c r="B13" s="68" t="s">
         <v>549</v>
       </c>
@@ -12533,7 +12734,7 @@
       <c r="J13" s="34"/>
     </row>
     <row r="14" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="124"/>
+      <c r="A14" s="126"/>
       <c r="B14" s="68" t="s">
         <v>551</v>
       </c>
@@ -12555,7 +12756,7 @@
       <c r="J14" s="34"/>
     </row>
     <row r="15" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="124"/>
+      <c r="A15" s="126"/>
       <c r="B15" s="68" t="s">
         <v>553</v>
       </c>
@@ -12577,7 +12778,7 @@
       <c r="J15" s="34"/>
     </row>
     <row r="16" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="124"/>
+      <c r="A16" s="126"/>
       <c r="B16" s="68" t="s">
         <v>555</v>
       </c>
@@ -12599,7 +12800,7 @@
       <c r="J16" s="34"/>
     </row>
     <row r="17" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="124"/>
+      <c r="A17" s="126"/>
       <c r="B17" s="68" t="s">
         <v>557</v>
       </c>
@@ -12621,7 +12822,7 @@
       <c r="J17" s="34"/>
     </row>
     <row r="18" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="124"/>
+      <c r="A18" s="126"/>
       <c r="B18" s="68" t="s">
         <v>559</v>
       </c>

</xml_diff>